<commit_message>
Refresh with Ken's latest workbook
</commit_message>
<xml_diff>
--- a/src/Planning/understand-options-azure-devops-environments-capacity-guide.xlsx
+++ b/src/Planning/understand-options-azure-devops-environments-capacity-guide.xlsx
@@ -1,30 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willy\OneDrive\_repos\Guidance\src\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ken.muse\Source\Repos\ALMRangers Guidance\src\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{2807C006-C69B-4AC9-8D01-14B79F4CDF28}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{B2CD11E7-C4ED-4C84-8FBA-E50379023EA9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988E16C4-3487-44E7-BFF3-7C4BB7FE4FFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="9180" windowWidth="21840" windowHeight="7272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server Scenarios" sheetId="1" r:id="rId1"/>
-    <sheet name="Hardware Configurations" sheetId="7" r:id="rId2"/>
-    <sheet name="Constants" sheetId="5" state="hidden" r:id="rId3"/>
+    <sheet name="Constants" sheetId="5" state="hidden" r:id="rId2"/>
+    <sheet name="Hardware Configurations" sheetId="7" r:id="rId3"/>
+    <sheet name="Additional Servers" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="Active_Branches">'Additional Servers'!$F$10</definedName>
     <definedName name="BEEF_FACTOR">'Server Scenarios'!$C$9</definedName>
-    <definedName name="C_NO">Constants!$B$21</definedName>
-    <definedName name="C_YES">Constants!$B$20</definedName>
+    <definedName name="C_NO">Constants!$B$22</definedName>
+    <definedName name="C_YES">Constants!$B$21</definedName>
+    <definedName name="CS_DEMO_CORES">Constants!$C$9</definedName>
+    <definedName name="CS_DEMO_RAM">Constants!$D$9</definedName>
+    <definedName name="CS_DEMO_USERS">Constants!$B$9</definedName>
+    <definedName name="CS_HIGH_CORES">Constants!$C$11</definedName>
+    <definedName name="CS_HIGH_RAM">Constants!$D$11</definedName>
+    <definedName name="CS_HIGH_USERS">Constants!$B$11</definedName>
+    <definedName name="CS_LOW_CORES">Constants!$C$10</definedName>
+    <definedName name="CS_LOW_RAM">Constants!$D$10</definedName>
+    <definedName name="CS_LOW_USERS">Constants!$B$10</definedName>
+    <definedName name="CS_STORAGE_FACTOR">Constants!$B$19</definedName>
+    <definedName name="Current_BranchTip">'Additional Servers'!$F$9</definedName>
+    <definedName name="Current_Storage">'Additional Servers'!$C$9</definedName>
     <definedName name="Current_Users">'Server Scenarios'!$C$7</definedName>
     <definedName name="DUAL_CURRENT_OK">'Server Scenarios'!$F$13</definedName>
     <definedName name="DUAL_FUTURE_OK">'Server Scenarios'!$F$14</definedName>
+    <definedName name="Future_BranchTip">'Additional Servers'!$F$8</definedName>
+    <definedName name="Future_Storage">'Additional Servers'!$C$8</definedName>
     <definedName name="Future_Users">'Server Scenarios'!$C$6</definedName>
+    <definedName name="GVFS_SCALE_FACTOR">Constants!$B$18</definedName>
     <definedName name="HI_CORE_AT">Constants!$F$5</definedName>
     <definedName name="HI_CORE_DT">Constants!$I$5</definedName>
     <definedName name="HI_DISK_AT">Constants!$H$5</definedName>
@@ -51,6 +68,15 @@
     <definedName name="MEDIUM_RPS">Constants!$B$4</definedName>
     <definedName name="MEDIUM_TPC">Constants!$E$4</definedName>
     <definedName name="MEDIUM_USERS">Constants!$C$4</definedName>
+    <definedName name="PROXY_HIGH_CORES">Constants!$C$16</definedName>
+    <definedName name="PROXY_HIGH_RAM">Constants!$D$16</definedName>
+    <definedName name="PROXY_HIGH_USERS">Constants!$B$16</definedName>
+    <definedName name="PROXY_LOW_CORES">Constants!$C$14</definedName>
+    <definedName name="PROXY_LOW_RAM">Constants!$D$14</definedName>
+    <definedName name="PROXY_LOW_USERS">Constants!$B$14</definedName>
+    <definedName name="PROXY_MEDIUM_CORES">Constants!$C$15</definedName>
+    <definedName name="PROXY_MEDIUM_RAM">Constants!$D$15</definedName>
+    <definedName name="PROXY_MEDIUM_USERS">Constants!$B$15</definedName>
     <definedName name="SCALE_CORE_AT">Constants!$F$6</definedName>
     <definedName name="SCALE_CORE_DT">Constants!$I$6</definedName>
     <definedName name="SCALE_CURRENT_OK">'Server Scenarios'!$I$13</definedName>
@@ -73,14 +99,22 @@
     <definedName name="STANDARD_RPD">Constants!$B$3</definedName>
     <definedName name="STANDARD_TPC">Constants!$E$3</definedName>
     <definedName name="STANDARD_USERS">Constants!$C$3</definedName>
-    <definedName name="VIRTUAL_PERCENTAGE">Constants!$B$19</definedName>
+    <definedName name="VM_OVERHEAD">Constants!$B$20</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="88">
   <si>
     <t>F</t>
   </si>
@@ -243,9 +277,6 @@
     </r>
   </si>
   <si>
-    <t>Visual Studio ALM Rangers - On-Premises Capacity Planning Quick Reference Poster Companion Workbook</t>
-  </si>
-  <si>
     <t>NUMBER OF ACTIVE TEAM FOUNDATION SERVER USERS</t>
   </si>
   <si>
@@ -273,9 +304,6 @@
     <t>RPS Factor</t>
   </si>
   <si>
-    <t>Estimated requests per second (rps) on AT server</t>
-  </si>
-  <si>
     <t>Estimated number of Application Tier (AT) servers</t>
   </si>
   <si>
@@ -291,12 +319,6 @@
     <t>Server Configuration Type</t>
   </si>
   <si>
-    <t>Estimated requests per second (rps) in total</t>
-  </si>
-  <si>
-    <t>Virtual Percentage</t>
-  </si>
-  <si>
     <t>RAM-DT</t>
   </si>
   <si>
@@ -313,9 +335,6 @@
   </si>
   <si>
     <t>DISK-DT</t>
-  </si>
-  <si>
-    <t>BETA</t>
   </si>
   <si>
     <t>Maximum expected users</t>
@@ -435,10 +454,103 @@
     </r>
   </si>
   <si>
-    <t>Version 2018.08.03</t>
-  </si>
-  <si>
     <t>Medium-End Configuration</t>
+  </si>
+  <si>
+    <t>Code Search Server</t>
+  </si>
+  <si>
+    <t>Standalone Server</t>
+  </si>
+  <si>
+    <t>Code Search Low-End</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>Code Search High-End</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Proxy Server</t>
+  </si>
+  <si>
+    <t>Standalone Server With GVFS</t>
+  </si>
+  <si>
+    <t>Search Server Storage</t>
+  </si>
+  <si>
+    <t>Proxy Low-End</t>
+  </si>
+  <si>
+    <t>Proxy Medium-End</t>
+  </si>
+  <si>
+    <t>Proxy High-End</t>
+  </si>
+  <si>
+    <t>Branch Tip Size (GB)</t>
+  </si>
+  <si>
+    <t>GVFS Storage Scale</t>
+  </si>
+  <si>
+    <t>ALM | DevOps Rangers - On-Premises Capacity Planning Quick Reference Poster Companion Workbook</t>
+  </si>
+  <si>
+    <t>Version 2019.04.21</t>
+  </si>
+  <si>
+    <t>Total Repository Size (GB)</t>
+  </si>
+  <si>
+    <t>Current recommendation is is 1.5x the repository's entire size</t>
+  </si>
+  <si>
+    <t>Current recommendation is 4x the repository's entire size</t>
+  </si>
+  <si>
+    <t>Code Search Demo</t>
+  </si>
+  <si>
+    <t>Configure</t>
+  </si>
+  <si>
+    <t>Co-located</t>
+  </si>
+  <si>
+    <t>Standalone</t>
+  </si>
+  <si>
+    <t>Users (From Server Scenarios)</t>
+  </si>
+  <si>
+    <t>Maximum Expected</t>
+  </si>
+  <si>
+    <t>Active Branches</t>
+  </si>
+  <si>
+    <t>Virtualization Overhead</t>
+  </si>
+  <si>
+    <t>Overhead for a system running on a virtual machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Maximum size must be less than current size</t>
+  </si>
+  <si>
+    <t>Maximum tip size must be greater than current tip size</t>
   </si>
   <si>
     <r>
@@ -453,7 +565,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>https://docs.microsoft.com/en-us/tfs/server/requirements</t>
+      <t>https://docs.microsoft.com/en-us/azure/devops/server/requirements</t>
     </r>
     <r>
       <rPr>
@@ -464,6 +576,48 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> for up-to-date operating system, hardware, virtualization, and other requirements.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Read </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://docs.microsoft.com/en-us/azure/devops/server/requirements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for up-to-date operating system, hardware, virtualization, and other requirements</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hardware requirements for Code Search can be found at </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://docs.microsoft.com/en-us/azure/devops/project/search/administration</t>
     </r>
   </si>
 </sst>
@@ -605,13 +759,6 @@
     </font>
     <font>
       <sz val="72"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="72"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -634,6 +781,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -689,7 +845,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -793,15 +949,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -992,11 +1139,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1004,9 +1189,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1014,10 +1198,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1029,75 +1213,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1111,56 +1261,55 @@
     <xf numFmtId="1" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1170,82 +1319,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1254,7 +1401,7 @@
     <xf numFmtId="0" fontId="16" fillId="4" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1263,12 +1410,9 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1281,10 +1425,10 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1302,23 +1446,109 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="4" tint="0.79998168889431442"/>
@@ -1378,61 +1608,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>381001</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2990938</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>899025</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="381001" y="4343400"/>
-          <a:ext cx="3219537" cy="1080000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1756,7 +1931,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -1764,391 +1939,319 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="19"/>
-    <col min="2" max="2" width="64.6640625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="9" style="19" customWidth="1"/>
-    <col min="4" max="4" width="3.33203125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="19" customWidth="1"/>
-    <col min="7" max="7" width="1.5546875" style="19" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="19" customWidth="1"/>
-    <col min="9" max="9" width="9" style="19" customWidth="1"/>
-    <col min="10" max="10" width="2.33203125" style="19" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" style="19" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="19"/>
+    <col min="2" max="2" width="64.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="3.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1"/>
+    <col min="7" max="7" width="1.5546875" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="2.33203125" customWidth="1"/>
+    <col min="11" max="11" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B1" s="20" t="s">
-        <v>26</v>
+      <c r="B1" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="71" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
+      <c r="B2" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
-        <v>54</v>
+      <c r="B3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="91" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="95" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="96"/>
-    </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="1.65">
-      <c r="A6" s="91"/>
-      <c r="B6" s="66" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="67">
-        <v>0</v>
-      </c>
-      <c r="D6" s="21" t="s">
+      <c r="A5" s="75" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="79" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="80"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="75"/>
+      <c r="B6" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="51">
+        <v>0</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="64" t="s">
+    </row>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="76"/>
+      <c r="B7" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="53">
+        <v>0</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="19"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="18"/>
+    </row>
+    <row r="9" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="19"/>
+      <c r="B9" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="E9" s="21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="92"/>
-      <c r="B7" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="69">
-        <v>0</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="21"/>
-    </row>
-    <row r="9" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="22"/>
-      <c r="B9" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="16">
-        <v>0.25</v>
-      </c>
-      <c r="E9" s="26" t="s">
-        <v>55</v>
-      </c>
-    </row>
     <row r="10" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="21"/>
+      <c r="A10" s="19"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="18"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="93" t="s">
+      <c r="B11" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="83" t="s">
+      <c r="C11" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="83"/>
-      <c r="E11" s="83"/>
-      <c r="F11" s="83" t="s">
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="83"/>
-      <c r="H11" s="83"/>
-      <c r="I11" s="83" t="s">
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="83"/>
-      <c r="K11" s="84"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="70"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="94"/>
-      <c r="C12" s="85" t="s">
+      <c r="B12" s="78"/>
+      <c r="C12" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="85"/>
-      <c r="E12" s="85"/>
-      <c r="F12" s="85" t="s">
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="85"/>
-      <c r="H12" s="85"/>
-      <c r="I12" s="85" t="s">
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="85"/>
-      <c r="K12" s="86"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="72"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="87" t="str">
+      <c r="C13" s="73" t="str">
         <f>IF(Current_Users&gt;STANDARD_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87" t="str">
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73" t="str">
         <f>IF(Current_Users&gt;HI_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="G13" s="87"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="87" t="str">
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73" t="str">
         <f>I14</f>
         <v>No</v>
       </c>
-      <c r="J13" s="87"/>
-      <c r="K13" s="88"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="74"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="89" t="str">
+      <c r="C14" s="73" t="str">
         <f>IF(Future_Users&gt;STANDARD_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="89" t="str">
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73" t="str">
         <f>IF(Future_Users&gt;HI_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="G14" s="89"/>
-      <c r="H14" s="89"/>
-      <c r="I14" s="89" t="str">
+      <c r="G14" s="73"/>
+      <c r="H14" s="73"/>
+      <c r="I14" s="73" t="str">
         <f>IF(Future_Users&gt;STANDARD_USERS,C_YES,C_NO)</f>
         <v>No</v>
       </c>
-      <c r="J14" s="89"/>
-      <c r="K14" s="90"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="74"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="89" t="str">
+      <c r="C15" s="73" t="str">
         <f>IF((COUNTIF(C13:C14,C_YES)&gt;1),C_YES,C_NO)</f>
         <v>Yes</v>
       </c>
-      <c r="D15" s="89"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89" t="str">
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73" t="str">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;1),C_YES,C_NO)</f>
         <v>Yes</v>
       </c>
-      <c r="G15" s="89"/>
-      <c r="H15" s="89"/>
-      <c r="I15" s="89" t="str">
+      <c r="G15" s="73"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="73" t="str">
         <f>IF((COUNTIF(I13:I14,C_YES)&gt;0),C_YES,C_NO)</f>
         <v>No</v>
       </c>
-      <c r="J15" s="89"/>
-      <c r="K15" s="90"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="74"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="29" t="str">
+      <c r="B16" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="24" t="str">
         <f>IF(C13=C_YES,(IF(Current_Users&gt;LO_USERS,"Standard","Low-End")),"")</f>
         <v>Low-End</v>
       </c>
-      <c r="D16" s="30" t="str">
+      <c r="D16" s="25" t="str">
         <f>IF(E16="","","-")</f>
         <v>-</v>
       </c>
-      <c r="E16" s="31" t="str">
+      <c r="E16" s="26" t="str">
         <f>IF(C14=C_YES,(IF(Future_Users&gt;LO_USERS,"Standard","Low-End")),"")</f>
         <v>Low-End</v>
       </c>
-      <c r="F16" s="72" t="str">
+      <c r="F16" s="63" t="str">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;0),"High-End","")</f>
         <v>High-End</v>
       </c>
-      <c r="G16" s="72"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="72" t="str">
+      <c r="G16" s="63"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="63" t="str">
         <f>IF((COUNTIF(I13:I14,C_YES)&gt;0),"Scale Unit","")</f>
         <v/>
       </c>
-      <c r="J16" s="72"/>
-      <c r="K16" s="73"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="64"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="74">
+      <c r="B17" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="65">
         <f>IF(C13=C_YES,(IF(Current_Users&gt;LO_USERS,STANDARD_TPC,LO_TPC)),"")</f>
         <v>5</v>
       </c>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74">
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65">
         <f>IF(F13=C_YES,HIGH_TPC,"")</f>
         <v>75</v>
       </c>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74" t="str">
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65" t="str">
         <f>IF(I13=C_YES,SCALE_TPC,"")</f>
         <v/>
       </c>
-      <c r="J17" s="74"/>
-      <c r="K17" s="79"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="66"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B18" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="80">
+      <c r="B18" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="67">
         <f>IF(C13=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_TPC,LO_TPC)),"")</f>
         <v>5</v>
       </c>
-      <c r="D18" s="80"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="74">
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="65">
         <f>IF(F14=C_YES,HIGH_TPC,"")</f>
         <v>75</v>
       </c>
-      <c r="G18" s="74"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="80" t="str">
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="67" t="str">
         <f>IF(I14=C_YES,SCALE_TPC,"")</f>
         <v/>
       </c>
-      <c r="J18" s="80"/>
-      <c r="K18" s="81"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="82">
+      <c r="J18" s="67"/>
+      <c r="K18" s="68"/>
+    </row>
+    <row r="19" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="61">
         <f>IF((COUNTIF(C13:C14,C_YES)&gt;0),1,"")</f>
         <v>1</v>
       </c>
-      <c r="D19" s="82"/>
-      <c r="E19" s="82"/>
-      <c r="F19" s="82">
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;0),1,"")</f>
         <v>1</v>
       </c>
-      <c r="G19" s="82"/>
-      <c r="H19" s="82"/>
-      <c r="I19" s="34" t="str">
-        <f>IF(I13=C_YES,ROUNDUP(I20/SCALE_RPS,0),"")</f>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="58" t="str">
+        <f>IF(I13=C_YES,ROUNDUP((Current_Users*SCALE_FACTOR)/SCALE_RPS,0),"")</f>
         <v/>
       </c>
-      <c r="J19" s="35" t="str">
+      <c r="J19" s="59" t="str">
         <f>IF(K19&lt;&gt;"","-","")</f>
         <v/>
       </c>
-      <c r="K19" s="36" t="str">
-        <f>IF(I14=C_YES,ROUNDUP(K20/SCALE_RPS,0),"")</f>
+      <c r="K19" s="60" t="str">
+        <f>IF(I14=C_YES,ROUNDUP((Future_Users*HI_FACTOR)/SCALE_RPS,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="75">
-        <f>IF(C13=C_YES,(IF(Current_Users&gt;LO_USERS,Current_Users*STANDARD_FACTOR,Current_Users*LO_FACTOR)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="D20" s="75" t="str">
-        <f>IF(E20&lt;&gt;"","-","")</f>
-        <v>-</v>
-      </c>
-      <c r="E20" s="75">
-        <f>IF(C14=C_YES,(IF(Future_Users&gt;LO_USERS,Future_Users*STANDARD_FACTOR,Future_Users*LO_FACTOR)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="77">
-        <f>IF(F13=C_YES,Current_Users*HI_FACTOR,"")</f>
-        <v>0</v>
-      </c>
-      <c r="G20" s="75" t="str">
-        <f>IF(H20&lt;&gt;"","-","")</f>
-        <v>-</v>
-      </c>
-      <c r="H20" s="77">
-        <f>IF(F14=C_YES,Future_Users*HI_FACTOR,"")</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="37" t="str">
-        <f>IF(I13=C_YES,Current_Users*SCALE_FACTOR,"")</f>
-        <v/>
-      </c>
-      <c r="J20" s="38" t="str">
-        <f>IF(K20&lt;&gt;"","-","")</f>
-        <v/>
-      </c>
-      <c r="K20" s="39" t="str">
-        <f>IF(I13=C_YES,Future_Users*HI_FACTOR,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="76"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="41" t="str">
-        <f>IF(I13=C_YES,I20/I19,"")</f>
-        <v/>
-      </c>
-      <c r="J21" s="42" t="str">
-        <f>IF(K21&lt;&gt;"","-","")</f>
-        <v/>
-      </c>
-      <c r="K21" s="43" t="str">
-        <f>IF(I14=C_YES,K20/K19,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="2:11" ht="91.8" x14ac:dyDescent="1.65">
-      <c r="B24" s="65"/>
+    <row r="22" spans="2:11" ht="91.8" x14ac:dyDescent="1.65">
+      <c r="B22" s="49"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="29">
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C17:E17"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="F12:H12"/>
@@ -2157,54 +2260,48 @@
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
     <mergeCell ref="I13:K13"/>
     <mergeCell ref="I14:K14"/>
     <mergeCell ref="I15:K15"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C15:E15"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="C17:E17"/>
   </mergeCells>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="7" priority="13">
+    <cfRule type="expression" dxfId="19" priority="13">
       <formula>$C$6&gt;=$C$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D8 D10">
-    <cfRule type="expression" dxfId="6" priority="12">
+    <cfRule type="expression" dxfId="18" priority="12">
       <formula>$C$7&lt;=$C$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:C15 F13:F16 I13:I16">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>$C$9&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -2238,11 +2335,397 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.21875" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="11" style="14" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="14">
+        <v>92</v>
+      </c>
+      <c r="C2" s="14">
+        <v>250</v>
+      </c>
+      <c r="D2">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E2" s="14">
+        <v>5</v>
+      </c>
+      <c r="F2" s="14">
+        <v>2</v>
+      </c>
+      <c r="G2" s="14">
+        <v>4</v>
+      </c>
+      <c r="H2" s="14">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="14">
+        <v>180</v>
+      </c>
+      <c r="C3" s="14">
+        <v>500</v>
+      </c>
+      <c r="D3">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E3" s="14">
+        <v>10</v>
+      </c>
+      <c r="F3" s="14">
+        <v>2</v>
+      </c>
+      <c r="G3" s="14">
+        <v>8</v>
+      </c>
+      <c r="H3" s="14">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="14">
+        <v>476</v>
+      </c>
+      <c r="C4" s="14">
+        <v>2000</v>
+      </c>
+      <c r="D4">
+        <v>0.21249999999999999</v>
+      </c>
+      <c r="E4" s="14">
+        <f>SCALE_TPC</f>
+        <v>75</v>
+      </c>
+      <c r="F4" s="14">
+        <v>2</v>
+      </c>
+      <c r="G4" s="14">
+        <v>8</v>
+      </c>
+      <c r="H4" s="14">
+        <v>500</v>
+      </c>
+      <c r="I4" s="14">
+        <v>4</v>
+      </c>
+      <c r="J4" s="14">
+        <v>8</v>
+      </c>
+      <c r="K4" s="14">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="14">
+        <v>730</v>
+      </c>
+      <c r="C5" s="14">
+        <v>3600</v>
+      </c>
+      <c r="D5">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="E5" s="14">
+        <v>75</v>
+      </c>
+      <c r="F5" s="14">
+        <v>4</v>
+      </c>
+      <c r="G5" s="14">
+        <v>16</v>
+      </c>
+      <c r="H5" s="14">
+        <v>500</v>
+      </c>
+      <c r="I5" s="14">
+        <v>8</v>
+      </c>
+      <c r="J5" s="14">
+        <v>16</v>
+      </c>
+      <c r="K5" s="14">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="14">
+        <v>476</v>
+      </c>
+      <c r="C6" s="14">
+        <v>2200</v>
+      </c>
+      <c r="D6">
+        <v>0.26250000000000001</v>
+      </c>
+      <c r="E6" s="14">
+        <v>75</v>
+      </c>
+      <c r="F6" s="14">
+        <v>2</v>
+      </c>
+      <c r="G6" s="14">
+        <v>8</v>
+      </c>
+      <c r="H6" s="14">
+        <v>500</v>
+      </c>
+      <c r="I6" s="14">
+        <v>8</v>
+      </c>
+      <c r="J6" s="14">
+        <v>16</v>
+      </c>
+      <c r="K6" s="14">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="54">
+        <v>250</v>
+      </c>
+      <c r="C9" s="54">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="14">
+        <v>500</v>
+      </c>
+      <c r="C10" s="14">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="14">
+        <v>1000</v>
+      </c>
+      <c r="C11" s="14">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="14">
+        <v>450</v>
+      </c>
+      <c r="C14" s="14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="14">
+        <v>2200</v>
+      </c>
+      <c r="C15" s="14">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="14">
+        <v>3600</v>
+      </c>
+      <c r="C16" s="14">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="29">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="56">
+        <v>1.5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="29">
+        <v>0.2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:M33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M2"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2255,944 +2738,934 @@
   <sheetData>
     <row r="1" spans="2:13" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="103" t="str">
+      <c r="B2" s="73" t="str">
         <f>'Server Scenarios'!B2:K2</f>
-        <v>Version 2018.08.03</v>
-      </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
+        <v>Version 2019.04.21</v>
+      </c>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="118" t="s">
-        <v>56</v>
+      <c r="B3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="97" t="s">
-        <v>52</v>
+      <c r="B6" s="81" t="s">
+        <v>47</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="111" t="s">
+      <c r="D6" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="112"/>
-      <c r="F6" s="111" t="s">
+      <c r="E6" s="95"/>
+      <c r="F6" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="113"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="113"/>
-      <c r="J6" s="111" t="s">
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="96"/>
+      <c r="J6" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="113"/>
-      <c r="L6" s="113"/>
-      <c r="M6" s="112"/>
+      <c r="K6" s="96"/>
+      <c r="L6" s="96"/>
+      <c r="M6" s="95"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="98"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="114" t="s">
+      <c r="F7" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="115"/>
-      <c r="H7" s="116" t="s">
+      <c r="G7" s="98"/>
+      <c r="H7" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="115"/>
-      <c r="J7" s="114" t="s">
+      <c r="I7" s="98"/>
+      <c r="J7" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="115"/>
-      <c r="L7" s="116" t="s">
+      <c r="K7" s="98"/>
+      <c r="L7" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="117"/>
+      <c r="M7" s="100"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="98"/>
+      <c r="B8" s="82"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="L8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="M8" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="98"/>
+      <c r="B9" s="82"/>
       <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="48">
+      <c r="D9" s="33">
         <f>IF(SINGLE_CURRENT_OK=C_YES,(IF(Current_Users&gt;LO_USERS,STANDARD_CORE_AT,LO_CORE_AT)),0)</f>
-        <v>1</v>
-      </c>
-      <c r="E9" s="50">
-        <f>IFD9+D9*VIRTUAL_PERCENTAGE</f>
-        <v>0.2</v>
-      </c>
-      <c r="F9" s="48">
+        <v>2</v>
+      </c>
+      <c r="E9" s="35">
+        <f>IFD9+D9*VM_OVERHEAD</f>
+        <v>0.4</v>
+      </c>
+      <c r="F9" s="33">
         <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_CORE_AT,MEDIUM_CORE_AT)),0)</f>
         <v>2</v>
       </c>
-      <c r="G9" s="51">
+      <c r="G9" s="36">
         <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_CORE_DT,MEDIUM_CORE_DT)),0)</f>
         <v>4</v>
       </c>
-      <c r="H9" s="52">
-        <f>F9+F9*VIRTUAL_PERCENTAGE</f>
+      <c r="H9" s="37">
+        <f>F9+F9*VM_OVERHEAD</f>
         <v>2.4</v>
       </c>
-      <c r="I9" s="17">
-        <f>IF(G9&lt;&gt;"",ROUNDUP(G9+G9*VIRTUAL_PERCENTAGE,0),0)</f>
+      <c r="I9" s="16">
+        <f>IF(G9&lt;&gt;"",ROUNDUP(G9+G9*VM_OVERHEAD,0),0)</f>
         <v>5</v>
       </c>
-      <c r="J9" s="48">
+      <c r="J9" s="33">
         <f>IF(SCALE_CURRENT_OK=C_YES,SCALE_CORE_AT,0)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="51">
+      <c r="K9" s="36">
         <f>IF(SCALE_CURRENT_OK=C_YES,(IF(Current_Users&gt;SCALE_USERS,SCALE_CORE_DT,SCALE_CORE_DT)),0)</f>
         <v>0</v>
       </c>
-      <c r="L9" s="52">
-        <f>J9+J9*VIRTUAL_PERCENTAGE</f>
-        <v>0</v>
-      </c>
-      <c r="M9" s="53">
-        <f>IF(K9&lt;&gt;"",ROUNDUP(K9+K9*VIRTUAL_PERCENTAGE,0),0)</f>
+      <c r="L9" s="37">
+        <f>J9+J9*VM_OVERHEAD</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="38">
+        <f>IF(K9&lt;&gt;"",ROUNDUP(K9+K9*VM_OVERHEAD,0),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="98"/>
+      <c r="B10" s="82"/>
       <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="48">
+      <c r="D10" s="33">
         <f>IF(SINGLE_CURRENT_OK=C_YES,(IF(Current_Users&gt;LO_USERS,STANDARD_RAM_AT,LO_RAM_AT)),0)</f>
         <v>4</v>
       </c>
-      <c r="E10" s="50">
-        <f>D10+D10*VIRTUAL_PERCENTAGE</f>
+      <c r="E10" s="35">
+        <f>D10+D10*VM_OVERHEAD</f>
         <v>4.8</v>
       </c>
-      <c r="F10" s="48">
+      <c r="F10" s="33">
         <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_RAM_AT,MEDIUM_RAM_AT)),0)</f>
         <v>8</v>
       </c>
-      <c r="G10" s="51">
+      <c r="G10" s="36">
         <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_RAM_DT,MEDIUM_RAM_DT)),0)</f>
         <v>8</v>
       </c>
-      <c r="H10" s="52">
-        <f>F10+F10*VIRTUAL_PERCENTAGE</f>
+      <c r="H10" s="37">
+        <f>F10+F10*VM_OVERHEAD</f>
         <v>9.6</v>
       </c>
-      <c r="I10" s="17">
-        <f>IF(G10&lt;&gt;"",ROUNDUP(G10+G10*VIRTUAL_PERCENTAGE,0),0)</f>
+      <c r="I10" s="16">
+        <f>IF(G10&lt;&gt;"",ROUNDUP(G10+G10*VM_OVERHEAD,0),0)</f>
         <v>10</v>
       </c>
-      <c r="J10" s="48">
+      <c r="J10" s="33">
         <f>IF(SCALE_CURRENT_OK=C_YES,SCALE_RAM_AT,0)</f>
         <v>0</v>
       </c>
-      <c r="K10" s="51">
+      <c r="K10" s="36">
         <f>IF(SCALE_CURRENT_OK=C_YES,(IF(Current_Users&gt;SCALE_USERS,SCALE_RAM_DT,SCALE_RAM_DT)),0)</f>
         <v>0</v>
       </c>
-      <c r="L10" s="52">
-        <f>J10+J10*VIRTUAL_PERCENTAGE</f>
-        <v>0</v>
-      </c>
-      <c r="M10" s="53">
-        <f>IF(K10&lt;&gt;"",ROUNDUP(K10+K10*VIRTUAL_PERCENTAGE,0),0)</f>
+      <c r="L10" s="37">
+        <f>J10+J10*VM_OVERHEAD</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="38">
+        <f>IF(K10&lt;&gt;"",ROUNDUP(K10+K10*VM_OVERHEAD,0),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="98"/>
+      <c r="B11" s="82"/>
       <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="49">
+      <c r="D11" s="34">
         <f>IF(SINGLE_CURRENT_OK=C_YES,(IF(Current_Users&gt;LO_USERS,STANDARD_DISK_AT,LO_DISK_AT)),0)</f>
         <v>125</v>
       </c>
-      <c r="E11" s="62">
-        <f>D11+D11*VIRTUAL_PERCENTAGE</f>
-        <v>150</v>
-      </c>
-      <c r="F11" s="49">
+      <c r="E11" s="47">
+        <f>D11</f>
+        <v>125</v>
+      </c>
+      <c r="F11" s="34">
         <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_DISK_AT,MEDIUM_DISK_AT)),0)</f>
         <v>500</v>
       </c>
-      <c r="G11" s="54">
+      <c r="G11" s="39">
         <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_DISK_DT,MEDIUM_DISK_DT)),0)</f>
         <v>2000</v>
       </c>
-      <c r="H11" s="63">
-        <f>F11+F11*VIRTUAL_PERCENTAGE</f>
-        <v>600</v>
-      </c>
-      <c r="I11" s="18">
-        <f>IF(G11&lt;&gt;"",ROUNDUP(G11+G11*VIRTUAL_PERCENTAGE,0),0)</f>
-        <v>2400</v>
-      </c>
-      <c r="J11" s="49">
+      <c r="H11" s="48">
+        <f>F11</f>
+        <v>500</v>
+      </c>
+      <c r="I11" s="17">
+        <f>IF(G11&lt;&gt;"",G11,0)</f>
+        <v>2000</v>
+      </c>
+      <c r="J11" s="34">
         <f>IF(SCALE_CURRENT_OK=C_YES,SCALE_DISK_AT,0)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="54">
+      <c r="K11" s="39">
         <f>IF(SCALE_CURRENT_OK=C_YES,(IF(Current_Users&gt;SCALE_USERS,SCALE_DISK_DT,SCALE_DISK_DT)),0)</f>
         <v>0</v>
       </c>
-      <c r="L11" s="63">
-        <f>J11+J11*VIRTUAL_PERCENTAGE</f>
-        <v>0</v>
-      </c>
-      <c r="M11" s="55">
-        <f>IF(K11&lt;&gt;"",ROUNDUP(K11+K11*VIRTUAL_PERCENTAGE,0),0)</f>
+      <c r="L11" s="48">
+        <f>J11</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="40">
+        <f>IF(K11&lt;&gt;"",K11,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="98"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
+      <c r="B12" s="82"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="98"/>
-      <c r="C13" s="45" t="s">
+      <c r="B13" s="82"/>
+      <c r="C13" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="104" t="s">
+      <c r="D13" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="105"/>
-      <c r="F13" s="104" t="s">
+      <c r="E13" s="88"/>
+      <c r="F13" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="106"/>
-      <c r="H13" s="106"/>
-      <c r="I13" s="106"/>
-      <c r="J13" s="104" t="s">
+      <c r="G13" s="89"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="89"/>
+      <c r="J13" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="106"/>
-      <c r="L13" s="106"/>
-      <c r="M13" s="105"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="88"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="98"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="56" t="s">
+      <c r="B14" s="82"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="57" t="s">
+      <c r="E14" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="107" t="s">
+      <c r="F14" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="108"/>
-      <c r="H14" s="109" t="s">
+      <c r="G14" s="91"/>
+      <c r="H14" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="108"/>
-      <c r="J14" s="107" t="s">
+      <c r="I14" s="91"/>
+      <c r="J14" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="108"/>
-      <c r="L14" s="109" t="s">
+      <c r="K14" s="91"/>
+      <c r="L14" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="110"/>
+      <c r="M14" s="93"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="98"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="56" t="s">
+      <c r="B15" s="82"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="57" t="s">
+      <c r="E15" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="56" t="s">
+      <c r="F15" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="58" t="s">
+      <c r="G15" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="59" t="s">
+      <c r="H15" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="58" t="s">
+      <c r="I15" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="56" t="s">
+      <c r="J15" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="58" t="s">
+      <c r="K15" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="L15" s="59" t="s">
+      <c r="L15" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="60" t="s">
+      <c r="M15" s="45" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="98"/>
-      <c r="C16" s="46" t="s">
+      <c r="B16" s="82"/>
+      <c r="C16" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D16" s="33">
         <f>IF(SINGLE_FUTURE_OK=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_CORE_AT,LO_CORE_AT)),0)</f>
-        <v>1</v>
-      </c>
-      <c r="E16" s="50">
-        <f>D16+D16*VIRTUAL_PERCENTAGE</f>
-        <v>1.2</v>
-      </c>
-      <c r="F16" s="48">
+        <v>2</v>
+      </c>
+      <c r="E16" s="35">
+        <f>D16+D16*VM_OVERHEAD</f>
+        <v>2.4</v>
+      </c>
+      <c r="F16" s="33">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_CORE_AT,MEDIUM_CORE_AT)),0)</f>
         <v>2</v>
       </c>
-      <c r="G16" s="51">
+      <c r="G16" s="36">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_CORE_DT,MEDIUM_CORE_DT)),0)</f>
         <v>4</v>
       </c>
-      <c r="H16" s="52">
-        <f>F16+F16*VIRTUAL_PERCENTAGE</f>
+      <c r="H16" s="37">
+        <f>F16+F16*VM_OVERHEAD</f>
         <v>2.4</v>
       </c>
-      <c r="I16" s="17">
-        <f>IF(G16&lt;&gt;"",ROUNDUP(G16+G16*VIRTUAL_PERCENTAGE,0),0)</f>
+      <c r="I16" s="16">
+        <f>IF(G16&lt;&gt;"",ROUNDUP(G16+G16*VM_OVERHEAD,0),0)</f>
         <v>5</v>
       </c>
-      <c r="J16" s="48">
+      <c r="J16" s="33">
         <f>IF(SCALE_FUTURE_OK=C_YES,SCALE_CORE_AT,0)</f>
         <v>0</v>
       </c>
-      <c r="K16" s="51">
+      <c r="K16" s="36">
         <f>IF(SCALE_FUTURE_OK=C_YES,(IF(Future_Users&gt;SCALE_USERS,SCALE_CORE_DT,SCALE_CORE_DT)),0)</f>
         <v>0</v>
       </c>
-      <c r="L16" s="52">
-        <f>J16+J16*VIRTUAL_PERCENTAGE</f>
-        <v>0</v>
-      </c>
-      <c r="M16" s="53">
-        <f>IF(K16&lt;&gt;"",ROUNDUP(K16+K16*VIRTUAL_PERCENTAGE,0),0)</f>
+      <c r="L16" s="37">
+        <f>J16+J16*VM_OVERHEAD</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="38">
+        <f>IF(K16&lt;&gt;"",ROUNDUP(K16+K16*VM_OVERHEAD,0),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="98"/>
-      <c r="C17" s="46" t="s">
+      <c r="B17" s="82"/>
+      <c r="C17" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="48">
+      <c r="D17" s="33">
         <f>IF(SINGLE_FUTURE_OK=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_RAM_AT,LO_RAM_AT)),0)</f>
         <v>4</v>
       </c>
-      <c r="E17" s="50">
-        <f>D17+D17*VIRTUAL_PERCENTAGE</f>
+      <c r="E17" s="35">
+        <f>D17+D17*VM_OVERHEAD</f>
         <v>4.8</v>
       </c>
-      <c r="F17" s="48">
+      <c r="F17" s="33">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_RAM_AT,MEDIUM_RAM_AT)),0)</f>
         <v>8</v>
       </c>
-      <c r="G17" s="51">
+      <c r="G17" s="36">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_RAM_DT,MEDIUM_RAM_DT)),0)</f>
         <v>8</v>
       </c>
-      <c r="H17" s="52">
-        <f>F17+F17*VIRTUAL_PERCENTAGE</f>
+      <c r="H17" s="37">
+        <f>F17+F17*VM_OVERHEAD</f>
         <v>9.6</v>
       </c>
-      <c r="I17" s="17">
-        <f>IF(G17&lt;&gt;"",ROUNDUP(G17+G17*VIRTUAL_PERCENTAGE,0),0)</f>
+      <c r="I17" s="16">
+        <f>IF(G17&lt;&gt;"",ROUNDUP(G17+G17*VM_OVERHEAD,0),0)</f>
         <v>10</v>
       </c>
-      <c r="J17" s="48">
+      <c r="J17" s="33">
         <f>IF(SCALE_FUTURE_OK=C_YES,SCALE_RAM_AT,0)</f>
         <v>0</v>
       </c>
-      <c r="K17" s="51">
+      <c r="K17" s="36">
         <f>IF(SCALE_FUTURE_OK=C_YES,(IF(Future_Users&gt;SCALE_USERS,SCALE_RAM_DT,SCALE_RAM_DT)),0)</f>
         <v>0</v>
       </c>
-      <c r="L17" s="52">
-        <f>J17+J17*VIRTUAL_PERCENTAGE</f>
-        <v>0</v>
-      </c>
-      <c r="M17" s="53">
-        <f>IF(K17&lt;&gt;"",ROUNDUP(K17+K17*VIRTUAL_PERCENTAGE,0),0)</f>
+      <c r="L17" s="37">
+        <f>J17+J17*VM_OVERHEAD</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="38">
+        <f>IF(K17&lt;&gt;"",ROUNDUP(K17+K17*VM_OVERHEAD,0),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="99"/>
-      <c r="C18" s="47" t="s">
+      <c r="B18" s="83"/>
+      <c r="C18" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="49">
+      <c r="D18" s="34">
         <f>IF(SINGLE_FUTURE_OK=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_DISK_AT,LO_DISK_AT)),0)</f>
         <v>125</v>
       </c>
-      <c r="E18" s="62">
-        <f>D18+D18*VIRTUAL_PERCENTAGE</f>
-        <v>150</v>
-      </c>
-      <c r="F18" s="49">
+      <c r="E18" s="47">
+        <f>D18</f>
+        <v>125</v>
+      </c>
+      <c r="F18" s="34">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,MEDIUM_DISK_AT,HI_DISK_AT)),0)</f>
         <v>500</v>
       </c>
-      <c r="G18" s="54">
+      <c r="G18" s="39">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_DISK_DT,MEDIUM_DISK_DT)),0)</f>
         <v>2000</v>
       </c>
-      <c r="H18" s="63">
-        <f>F18+F18*VIRTUAL_PERCENTAGE</f>
-        <v>600</v>
-      </c>
-      <c r="I18" s="18">
-        <f>IF(G18&lt;&gt;"",ROUNDUP(G18+G18*VIRTUAL_PERCENTAGE,0),0)</f>
-        <v>2400</v>
-      </c>
-      <c r="J18" s="49">
+      <c r="H18" s="48">
+        <f>F18</f>
+        <v>500</v>
+      </c>
+      <c r="I18" s="17">
+        <f>IF(G18&lt;&gt;"",G18,0)</f>
+        <v>2000</v>
+      </c>
+      <c r="J18" s="34">
         <f>IF(SCALE_FUTURE_OK=C_YES,SCALE_DISK_AT,0)</f>
         <v>0</v>
       </c>
-      <c r="K18" s="54">
+      <c r="K18" s="39">
         <f>IF(SCALE_FUTURE_OK=C_YES,(IF(Future_Users&gt;SCALE_USERS,SCALE_DISK_DT,SCALE_DISK_DT)),0)</f>
         <v>0</v>
       </c>
-      <c r="L18" s="63">
-        <f>J18+J18*VIRTUAL_PERCENTAGE</f>
-        <v>0</v>
-      </c>
-      <c r="M18" s="55">
-        <f>IF(K18&lt;&gt;"",ROUNDUP(K18+K18*VIRTUAL_PERCENTAGE,0),0)</f>
+      <c r="L18" s="48">
+        <f>J18</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="40">
+        <f>IF(K18&lt;&gt;"",K18,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="100" t="s">
-        <v>53</v>
+      <c r="B21" s="84" t="s">
+        <v>48</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="104" t="s">
+      <c r="D21" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="105"/>
-      <c r="F21" s="104" t="s">
+      <c r="E21" s="88"/>
+      <c r="F21" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="106"/>
-      <c r="H21" s="106"/>
-      <c r="I21" s="105"/>
-      <c r="J21" s="104" t="s">
+      <c r="G21" s="89"/>
+      <c r="H21" s="89"/>
+      <c r="I21" s="88"/>
+      <c r="J21" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="K21" s="106"/>
-      <c r="L21" s="106"/>
-      <c r="M21" s="105"/>
+      <c r="K21" s="89"/>
+      <c r="L21" s="89"/>
+      <c r="M21" s="88"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="101"/>
+      <c r="B22" s="85"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="56" t="s">
+      <c r="D22" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="57" t="s">
+      <c r="E22" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="107" t="s">
+      <c r="F22" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="108"/>
-      <c r="H22" s="109" t="s">
+      <c r="G22" s="91"/>
+      <c r="H22" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="110"/>
-      <c r="J22" s="107" t="s">
+      <c r="I22" s="93"/>
+      <c r="J22" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="108"/>
-      <c r="L22" s="109" t="s">
+      <c r="K22" s="91"/>
+      <c r="L22" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="M22" s="110"/>
+      <c r="M22" s="93"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="101"/>
+      <c r="B23" s="85"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="56" t="s">
+      <c r="D23" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="57" t="s">
+      <c r="E23" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="56" t="s">
+      <c r="F23" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="58" t="s">
+      <c r="G23" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="H23" s="59" t="s">
+      <c r="H23" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="I23" s="60" t="s">
+      <c r="I23" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="J23" s="56" t="s">
+      <c r="J23" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="K23" s="58" t="s">
+      <c r="K23" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="L23" s="59" t="s">
+      <c r="L23" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="M23" s="60" t="s">
+      <c r="M23" s="45" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="101"/>
+      <c r="B24" s="85"/>
       <c r="C24" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="48">
+      <c r="D24" s="33">
         <f t="shared" ref="D24:M24" si="0">ROUNDUP(D9+D9*BEEF_FACTOR,0)</f>
-        <v>2</v>
-      </c>
-      <c r="E24" s="50">
+        <v>3</v>
+      </c>
+      <c r="E24" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F24" s="48">
+      <c r="F24" s="33">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G24" s="17">
+      <c r="G24" s="16">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H24" s="52">
+      <c r="H24" s="37">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I24" s="53">
+      <c r="I24" s="38">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J24" s="48">
+      <c r="J24" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K24" s="17">
+      <c r="K24" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L24" s="52">
+      <c r="L24" s="37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M24" s="53">
+      <c r="M24" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="101"/>
+      <c r="B25" s="85"/>
       <c r="C25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="48">
+      <c r="D25" s="33">
         <f t="shared" ref="D25:M25" si="1">ROUNDUP(D10+D10*BEEF_FACTOR,0)</f>
         <v>5</v>
       </c>
-      <c r="E25" s="50">
+      <c r="E25" s="35">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="F25" s="48">
+      <c r="F25" s="33">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="G25" s="17">
+      <c r="G25" s="16">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="H25" s="52">
+      <c r="H25" s="37">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I25" s="53">
+      <c r="I25" s="38">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="J25" s="48">
+      <c r="J25" s="33">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K25" s="17">
+      <c r="K25" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L25" s="52">
+      <c r="L25" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M25" s="53">
+      <c r="M25" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="101"/>
+      <c r="B26" s="85"/>
       <c r="C26" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="49">
+      <c r="D26" s="34">
         <f t="shared" ref="D26:M26" si="2">ROUNDUP(D11+D11*BEEF_FACTOR,0)</f>
         <v>157</v>
       </c>
-      <c r="E26" s="62">
+      <c r="E26" s="47">
         <f t="shared" si="2"/>
-        <v>188</v>
-      </c>
-      <c r="F26" s="49">
+        <v>157</v>
+      </c>
+      <c r="F26" s="34">
         <f t="shared" si="2"/>
         <v>625</v>
       </c>
-      <c r="G26" s="18">
+      <c r="G26" s="17">
         <f t="shared" si="2"/>
         <v>2500</v>
       </c>
-      <c r="H26" s="63">
+      <c r="H26" s="48">
         <f t="shared" si="2"/>
-        <v>750</v>
-      </c>
-      <c r="I26" s="55">
+        <v>625</v>
+      </c>
+      <c r="I26" s="40">
         <f t="shared" si="2"/>
-        <v>3000</v>
-      </c>
-      <c r="J26" s="49">
+        <v>2500</v>
+      </c>
+      <c r="J26" s="34">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K26" s="18">
+      <c r="K26" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L26" s="63">
+      <c r="L26" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M26" s="55">
+      <c r="M26" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="101"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="61"/>
-      <c r="M27" s="61"/>
+      <c r="B27" s="85"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="101"/>
+      <c r="B28" s="85"/>
       <c r="C28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="104" t="s">
+      <c r="D28" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="105"/>
-      <c r="F28" s="104" t="s">
+      <c r="E28" s="88"/>
+      <c r="F28" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="G28" s="106"/>
-      <c r="H28" s="106"/>
-      <c r="I28" s="105"/>
-      <c r="J28" s="104" t="s">
+      <c r="G28" s="89"/>
+      <c r="H28" s="89"/>
+      <c r="I28" s="88"/>
+      <c r="J28" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="K28" s="106"/>
-      <c r="L28" s="106"/>
-      <c r="M28" s="105"/>
+      <c r="K28" s="89"/>
+      <c r="L28" s="89"/>
+      <c r="M28" s="88"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B29" s="101"/>
+      <c r="B29" s="85"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="56" t="s">
+      <c r="D29" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="57" t="s">
+      <c r="E29" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="F29" s="107" t="s">
+      <c r="F29" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="108"/>
-      <c r="H29" s="109" t="s">
+      <c r="G29" s="91"/>
+      <c r="H29" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="I29" s="110"/>
-      <c r="J29" s="107" t="s">
+      <c r="I29" s="93"/>
+      <c r="J29" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="K29" s="108"/>
-      <c r="L29" s="109" t="s">
+      <c r="K29" s="91"/>
+      <c r="L29" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="M29" s="110"/>
+      <c r="M29" s="93"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="101"/>
+      <c r="B30" s="85"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="56" t="s">
+      <c r="D30" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="57" t="s">
+      <c r="E30" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="F30" s="56" t="s">
+      <c r="F30" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="G30" s="58" t="s">
+      <c r="G30" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="H30" s="59" t="s">
+      <c r="H30" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="I30" s="60" t="s">
+      <c r="I30" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="J30" s="56" t="s">
+      <c r="J30" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="K30" s="58" t="s">
+      <c r="K30" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="L30" s="59" t="s">
+      <c r="L30" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="M30" s="60" t="s">
+      <c r="M30" s="45" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="101"/>
+      <c r="B31" s="85"/>
       <c r="C31" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="48">
+      <c r="D31" s="33">
         <f t="shared" ref="D31:M31" si="3">ROUNDUP(D16+D16*BEEF_FACTOR,0)</f>
-        <v>2</v>
-      </c>
-      <c r="E31" s="50">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="F31" s="48">
+        <v>3</v>
+      </c>
+      <c r="E31" s="35">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="G31" s="17">
+      <c r="F31" s="33">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G31" s="16">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="H31" s="52">
+      <c r="H31" s="37">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="I31" s="53">
+      <c r="I31" s="38">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="J31" s="48">
+      <c r="J31" s="33">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K31" s="17">
+      <c r="K31" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L31" s="52">
+      <c r="L31" s="37">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M31" s="53">
+      <c r="M31" s="38">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B32" s="101"/>
+      <c r="B32" s="85"/>
       <c r="C32" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="48">
+      <c r="D32" s="33">
         <f t="shared" ref="D32:M32" si="4">ROUNDUP(D17+D17*BEEF_FACTOR,0)</f>
         <v>5</v>
       </c>
-      <c r="E32" s="50">
+      <c r="E32" s="35">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="F32" s="48">
+      <c r="F32" s="33">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="G32" s="17">
+      <c r="G32" s="16">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="H32" s="52">
+      <c r="H32" s="37">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="I32" s="53">
+      <c r="I32" s="38">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="J32" s="48">
+      <c r="J32" s="33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K32" s="17">
+      <c r="K32" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L32" s="52">
+      <c r="L32" s="37">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M32" s="53">
+      <c r="M32" s="38">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="102"/>
+      <c r="B33" s="86"/>
       <c r="C33" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="49">
+      <c r="D33" s="34">
         <f t="shared" ref="D33:M33" si="5">ROUNDUP(D18+D18*BEEF_FACTOR,0)</f>
         <v>157</v>
       </c>
-      <c r="E33" s="62">
+      <c r="E33" s="47">
         <f t="shared" si="5"/>
-        <v>188</v>
-      </c>
-      <c r="F33" s="49">
+        <v>157</v>
+      </c>
+      <c r="F33" s="34">
         <f t="shared" si="5"/>
         <v>625</v>
       </c>
-      <c r="G33" s="18">
+      <c r="G33" s="17">
         <f t="shared" si="5"/>
         <v>2500</v>
       </c>
-      <c r="H33" s="63">
+      <c r="H33" s="48">
         <f t="shared" si="5"/>
-        <v>750</v>
-      </c>
-      <c r="I33" s="55">
+        <v>625</v>
+      </c>
+      <c r="I33" s="40">
         <f t="shared" si="5"/>
-        <v>3000</v>
-      </c>
-      <c r="J33" s="49">
+        <v>2500</v>
+      </c>
+      <c r="J33" s="34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K33" s="18">
+      <c r="K33" s="17">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L33" s="63">
+      <c r="L33" s="48">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M33" s="55">
+      <c r="M33" s="40">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3233,7 +3706,7 @@
     <mergeCell ref="J22:K22"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:M33">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3242,239 +3715,657 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K21"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B24151-BCDB-4D54-B778-984CD476EECE}">
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" customWidth="1"/>
-    <col min="2" max="3" width="11" style="15" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="15"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" customWidth="1"/>
+    <col min="9" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="15">
-        <v>92</v>
-      </c>
-      <c r="C2" s="15">
-        <v>250</v>
-      </c>
-      <c r="D2">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="E2" s="15">
-        <v>5</v>
-      </c>
-      <c r="F2" s="15">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="73" t="str">
+        <f>'Server Scenarios'!B2:K2</f>
+        <v>Version 2019.04.21</v>
+      </c>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="75" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="106"/>
+      <c r="D7" s="116" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="106"/>
+      <c r="H7" s="105" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="106"/>
+    </row>
+    <row r="8" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="75"/>
+      <c r="B8" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="51">
+        <v>0</v>
+      </c>
+      <c r="D8" s="116"/>
+      <c r="E8" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="51">
+        <v>0</v>
+      </c>
+      <c r="H8" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="I8" s="118">
+        <f>Future_Users</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="76"/>
+      <c r="B9" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="53">
+        <v>0</v>
+      </c>
+      <c r="D9" s="116"/>
+      <c r="E9" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="51">
+        <v>0</v>
+      </c>
+      <c r="H9" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="117">
+        <f>Current_Users</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E10" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="53">
         <v>1</v>
       </c>
-      <c r="G2" s="15">
-        <v>4</v>
-      </c>
-      <c r="H2" s="15">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="15">
-        <v>180</v>
-      </c>
-      <c r="C3" s="15">
-        <v>500</v>
-      </c>
-      <c r="D3">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="E3" s="15">
-        <v>10</v>
-      </c>
-      <c r="F3" s="15">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="104" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="113" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="114"/>
+      <c r="E13" s="114"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="94" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="95"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="82"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="103"/>
+      <c r="G14" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="82"/>
+      <c r="C15" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="108"/>
+      <c r="E15" s="108"/>
+      <c r="F15" s="109"/>
+      <c r="G15" s="33">
+        <f>IF(Current_Users&gt;CS_LOW_USERS,CS_HIGH_CORES,CS_LOW_CORES)</f>
         <v>2</v>
       </c>
-      <c r="G3" s="15">
+      <c r="H15" s="35">
+        <f>G15*(1+VM_OVERHEAD)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="82"/>
+      <c r="C16" s="107" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="108"/>
+      <c r="E16" s="108"/>
+      <c r="F16" s="109"/>
+      <c r="G16" s="33">
+        <f>IF(Current_Users&gt;CS_LOW_USERS,CS_HIGH_RAM,CS_LOW_RAM)</f>
         <v>8</v>
       </c>
-      <c r="H3" s="15">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="15">
-        <v>476</v>
-      </c>
-      <c r="C4" s="15">
-        <v>2200</v>
-      </c>
-      <c r="D4">
-        <v>0.21249999999999999</v>
-      </c>
-      <c r="E4" s="15">
-        <f>SCALE_TPC</f>
-        <v>75</v>
-      </c>
-      <c r="F4" s="15">
+      <c r="H16" s="35">
+        <f>G16*(1+VM_OVERHEAD)</f>
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="82"/>
+      <c r="C17" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="111"/>
+      <c r="E17" s="111"/>
+      <c r="F17" s="112"/>
+      <c r="G17" s="34">
+        <f>Current_Storage*CS_STORAGE_FACTOR</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="47">
+        <f>G17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="82"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="82"/>
+      <c r="C19" s="113" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="114"/>
+      <c r="E19" s="114"/>
+      <c r="F19" s="115"/>
+      <c r="G19" s="94" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="95"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B20" s="82"/>
+      <c r="C20" s="101"/>
+      <c r="D20" s="102"/>
+      <c r="E20" s="102"/>
+      <c r="F20" s="103"/>
+      <c r="G20" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B21" s="82"/>
+      <c r="C21" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="108"/>
+      <c r="E21" s="108"/>
+      <c r="F21" s="109"/>
+      <c r="G21" s="33">
+        <f>IF(Future_Users&gt;CS_LOW_USERS,CS_HIGH_CORES,CS_LOW_CORES)</f>
         <v>2</v>
       </c>
-      <c r="G4" s="15">
+      <c r="H21" s="35">
+        <f>G21*(1+VM_OVERHEAD)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B22" s="82"/>
+      <c r="C22" s="107" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="108"/>
+      <c r="E22" s="108"/>
+      <c r="F22" s="109"/>
+      <c r="G22" s="33">
+        <f>IF(Future_Users&gt;CS_LOW_USERS,CS_HIGH_RAM,CS_LOW_RAM)</f>
         <v>8</v>
       </c>
-      <c r="H4" s="15">
-        <v>500</v>
-      </c>
-      <c r="I4" s="15">
-        <v>4</v>
-      </c>
-      <c r="J4" s="15">
-        <v>8</v>
-      </c>
-      <c r="K4" s="15">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="15">
-        <v>730</v>
-      </c>
-      <c r="C5" s="15">
-        <v>3600</v>
-      </c>
-      <c r="D5">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="E5" s="15">
-        <v>75</v>
-      </c>
-      <c r="F5" s="15">
-        <v>4</v>
-      </c>
-      <c r="G5" s="15">
-        <v>16</v>
-      </c>
-      <c r="H5" s="15">
-        <v>500</v>
-      </c>
-      <c r="I5" s="15">
-        <v>8</v>
-      </c>
-      <c r="J5" s="15">
-        <v>16</v>
-      </c>
-      <c r="K5" s="15">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="15">
-        <v>476</v>
-      </c>
-      <c r="C6" s="15">
-        <v>2200</v>
-      </c>
-      <c r="D6">
-        <v>0.26250000000000001</v>
-      </c>
-      <c r="E6" s="15">
-        <v>75</v>
-      </c>
-      <c r="F6" s="15">
+      <c r="H22" s="35">
+        <f>G22*(1+VM_OVERHEAD)</f>
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="83"/>
+      <c r="C23" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="111"/>
+      <c r="E23" s="111"/>
+      <c r="F23" s="112"/>
+      <c r="G23" s="34">
+        <f>Future_Storage*CS_STORAGE_FACTOR</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="47">
+        <f>G23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B25" s="104" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="113" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="114"/>
+      <c r="E25" s="114"/>
+      <c r="F25" s="115"/>
+      <c r="G25" s="94" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" s="95"/>
+      <c r="I25" s="94" t="s">
+        <v>61</v>
+      </c>
+      <c r="J25" s="95"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B26" s="82"/>
+      <c r="C26" s="101"/>
+      <c r="D26" s="102"/>
+      <c r="E26" s="102"/>
+      <c r="F26" s="103"/>
+      <c r="G26" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="J26" s="42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="82"/>
+      <c r="C27" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="108"/>
+      <c r="E27" s="108"/>
+      <c r="F27" s="109"/>
+      <c r="G27" s="33">
+        <f>IF(Current_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Current_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
+        <v>1</v>
+      </c>
+      <c r="H27" s="35">
+        <f>G27*(1+VM_OVERHEAD)</f>
+        <v>1.2</v>
+      </c>
+      <c r="I27" s="33">
+        <f>IF(Current_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Current_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
+        <v>1</v>
+      </c>
+      <c r="J27" s="35">
+        <f>I27*(1+VM_OVERHEAD)</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B28" s="82"/>
+      <c r="C28" s="107" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="108"/>
+      <c r="E28" s="108"/>
+      <c r="F28" s="109"/>
+      <c r="G28" s="33">
+        <f>IF(Current_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_RAM, IF(Current_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_RAM,PROXY_MEDIUM_RAM))</f>
         <v>2</v>
       </c>
-      <c r="G6" s="15">
-        <v>8</v>
-      </c>
-      <c r="H6" s="15">
-        <v>500</v>
-      </c>
-      <c r="I6" s="70">
-        <v>8</v>
-      </c>
-      <c r="J6" s="70">
-        <v>16</v>
-      </c>
-      <c r="K6" s="70">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="44">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B21" s="15" t="s">
-        <v>22</v>
+      <c r="H28" s="35">
+        <f>G28*(1+VM_OVERHEAD)</f>
+        <v>2.4</v>
+      </c>
+      <c r="I28" s="33">
+        <f>G28+(Current_BranchTip)</f>
+        <v>2</v>
+      </c>
+      <c r="J28" s="35">
+        <f>I28*(1+VM_OVERHEAD)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="82"/>
+      <c r="C29" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="111"/>
+      <c r="E29" s="111"/>
+      <c r="F29" s="112"/>
+      <c r="G29" s="34">
+        <f>Current_BranchTip*Active_Branches</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="47">
+        <f>G29</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="34">
+        <f>Current_Storage*GVFS_SCALE_FACTOR</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="47">
+        <f>I29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="82"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B31" s="82"/>
+      <c r="C31" s="113" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="114"/>
+      <c r="E31" s="114"/>
+      <c r="F31" s="115"/>
+      <c r="G31" s="94" t="s">
+        <v>54</v>
+      </c>
+      <c r="H31" s="95"/>
+      <c r="I31" s="94" t="s">
+        <v>61</v>
+      </c>
+      <c r="J31" s="95"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B32" s="82"/>
+      <c r="C32" s="101"/>
+      <c r="D32" s="102"/>
+      <c r="E32" s="102"/>
+      <c r="F32" s="103"/>
+      <c r="G32" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" s="42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B33" s="82"/>
+      <c r="C33" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="108"/>
+      <c r="E33" s="108"/>
+      <c r="F33" s="109"/>
+      <c r="G33" s="33">
+        <f>IF(Future_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Future_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
+        <v>1</v>
+      </c>
+      <c r="H33" s="35">
+        <f>G33*(1+VM_OVERHEAD)</f>
+        <v>1.2</v>
+      </c>
+      <c r="I33" s="33">
+        <f>IF(Future_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Future_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
+        <v>1</v>
+      </c>
+      <c r="J33" s="35">
+        <f>I33*(1+VM_OVERHEAD)</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B34" s="82"/>
+      <c r="C34" s="107" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="108"/>
+      <c r="E34" s="108"/>
+      <c r="F34" s="109"/>
+      <c r="G34" s="33">
+        <f>IF(Future_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_RAM, IF(Future_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_RAM,PROXY_MEDIUM_RAM))</f>
+        <v>2</v>
+      </c>
+      <c r="H34" s="35">
+        <f>G34*(1+VM_OVERHEAD)</f>
+        <v>2.4</v>
+      </c>
+      <c r="I34" s="33">
+        <f>G34+Future_BranchTip</f>
+        <v>2</v>
+      </c>
+      <c r="J34" s="35">
+        <f>I34*(1+VM_OVERHEAD)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="83"/>
+      <c r="C35" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="111"/>
+      <c r="E35" s="111"/>
+      <c r="F35" s="112"/>
+      <c r="G35" s="34">
+        <f>Future_BranchTip*Active_Branches</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="47">
+        <f>G35</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="34">
+        <f>Future_Storage*GVFS_SCALE_FACTOR</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="47">
+        <f>I35</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="34">
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B25:B35"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C29:F29"/>
+  </mergeCells>
+  <conditionalFormatting sqref="G13:H24">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G32:H35 G26:H30">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G25:H25">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G31:H31">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26:J26 J27:J29">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25:J25">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32:J32 J33:J35">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I33:I35">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31:J31">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27:I29">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>Current_Storage&lt;=Future_Storage</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>Current_BranchTip &lt;= Future_BranchTip</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <Project xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3">45</Project>
+    <Priority xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3">2 - Cheat sheet / posters (high)</Priority>
+    <Notes0 xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3" xsi:nil="true"/>
+    <Review_x0020_Status xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3">Review Completed</Review_x0020_Status>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CC8AB984F9AFA14087035BD77D90A626" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="587f6fb58f55cab20468d5767da9b76d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="d4f1fd26-cd3f-48df-8559-6269d85163e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d45bfae41b7a5cd5eac582b346e06dc" ns1:_="">
     <xsd:import namespace="d4f1fd26-cd3f-48df-8559-6269d85163e3"/>
@@ -3563,27 +4454,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <Project xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3">45</Project>
-    <Priority xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3">2 - Cheat sheet / posters (high)</Priority>
-    <Notes0 xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3" xsi:nil="true"/>
-    <Review_x0020_Status xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3">Review Completed</Review_x0020_Status>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{312B28CD-EB51-4560-8E58-B9E03DAFD80D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d4f1fd26-cd3f-48df-8559-6269d85163e3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13C0D350-2871-401C-8D5C-791C478D9E13}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E2C743B-52BB-4B93-BC7B-301A591373EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3598,21 +4492,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{312B28CD-EB51-4560-8E58-B9E03DAFD80D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d4f1fd26-cd3f-48df-8559-6269d85163e3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13C0D350-2871-401C-8D5C-791C478D9E13}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add instructions to spreadsheets
</commit_message>
<xml_diff>
--- a/src/Planning/understand-options-azure-devops-environments-capacity-guide.xlsx
+++ b/src/Planning/understand-options-azure-devops-environments-capacity-guide.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ken.muse\Source\Repos\ALMRangers Guidance\src\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ken.muse\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988E16C4-3487-44E7-BFF3-7C4BB7FE4FFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{91AF45C8-2D9E-4696-8D1D-8977D2C692C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,10 +16,10 @@
     <sheet name="Server Scenarios" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="5" state="hidden" r:id="rId2"/>
     <sheet name="Hardware Configurations" sheetId="7" r:id="rId3"/>
-    <sheet name="Additional Servers" sheetId="8" r:id="rId4"/>
+    <sheet name="Proxy Server" sheetId="8" r:id="rId4"/>
+    <sheet name="Code Search Server" sheetId="9" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="Active_Branches">'Additional Servers'!$F$10</definedName>
     <definedName name="BEEF_FACTOR">'Server Scenarios'!$C$9</definedName>
     <definedName name="C_NO">Constants!$B$22</definedName>
     <definedName name="C_YES">Constants!$B$21</definedName>
@@ -33,13 +33,15 @@
     <definedName name="CS_LOW_RAM">Constants!$D$10</definedName>
     <definedName name="CS_LOW_USERS">Constants!$B$10</definedName>
     <definedName name="CS_STORAGE_FACTOR">Constants!$B$19</definedName>
-    <definedName name="Current_BranchTip">'Additional Servers'!$F$9</definedName>
-    <definedName name="Current_Storage">'Additional Servers'!$C$9</definedName>
+    <definedName name="Current_BranchTip">'Proxy Server'!$F$8</definedName>
+    <definedName name="Current_Storage" localSheetId="4">'Code Search Server'!$C$9</definedName>
+    <definedName name="Current_Storage">'Proxy Server'!$C$8</definedName>
     <definedName name="Current_Users">'Server Scenarios'!$C$7</definedName>
     <definedName name="DUAL_CURRENT_OK">'Server Scenarios'!$F$13</definedName>
     <definedName name="DUAL_FUTURE_OK">'Server Scenarios'!$F$14</definedName>
-    <definedName name="Future_BranchTip">'Additional Servers'!$F$8</definedName>
-    <definedName name="Future_Storage">'Additional Servers'!$C$8</definedName>
+    <definedName name="Future_BranchTip">'Proxy Server'!$F$7</definedName>
+    <definedName name="Future_Storage" localSheetId="4">'Code Search Server'!$C$8</definedName>
+    <definedName name="Future_Storage">'Proxy Server'!$C$7</definedName>
     <definedName name="Future_Users">'Server Scenarios'!$C$6</definedName>
     <definedName name="GVFS_SCALE_FACTOR">Constants!$B$18</definedName>
     <definedName name="HI_CORE_AT">Constants!$F$5</definedName>
@@ -114,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="91">
   <si>
     <t>F</t>
   </si>
@@ -277,9 +279,6 @@
     </r>
   </si>
   <si>
-    <t>NUMBER OF ACTIVE TEAM FOUNDATION SERVER USERS</t>
-  </si>
-  <si>
     <t>Low-End Configuration</t>
   </si>
   <si>
@@ -535,9 +534,6 @@
     <t>Maximum Expected</t>
   </si>
   <si>
-    <t>Active Branches</t>
-  </si>
-  <si>
     <t>Virtualization Overhead</t>
   </si>
   <si>
@@ -618,6 +614,180 @@
         <scheme val="minor"/>
       </rPr>
       <t>https://docs.microsoft.com/en-us/azure/devops/project/search/administration</t>
+    </r>
+  </si>
+  <si>
+    <t>INSTRUCTIONS</t>
+  </si>
+  <si>
+    <t>NUMBER OF ACTIVE AZURE DEVOPS SERVER USERS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To use this simplified capacity planning tool, enter the maximum number of users expected to be actively using the Azure DevOps servers. Then, enter the current number of users for the system. The Infrastructure Architecture table will automatically update to indicate suggested server configurations. The tab </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hardware Configurations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> will contain the suggested minimum hardware specifications for the servers.
+If the one or more teams will be operating remotely and using Team Foundation Version Control (TFVC) or Git Virtual File System (GVFS), then consider using an Azure DevOps Proxy server to improve the performance. This can be configured using the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Proxy Server</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tab.
+To enable full-text search across Code, Wiki, packages, and work items, a Code Search Server will be required. This can be configured on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Code Search</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tab.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To estimate the requirements for the Code Search Server, enter the current and maximum expected repository size. The hardware requirements will be reflected in the table above.  If you're working with a Git repository, you can estimate the size by issuing the following commands and reviewing the value of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>size-pack</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>git gc
+git count-objects -vH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To estimate the required configuration for the Proxy Server, enter the current and expected maximum size of all code repositories which will be accessed. If you're working with a Git repository, you can estimate the size by issuing the following commands and reviewing the value of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>size-pack</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">git gc
+git count-objects -vH
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Additionally, enter the current and expected maximum tip sizes for all active branches. This is the size of the files in each active branch as queried from the file system.
+If the Git Virtual File System (GVFS) proxy feature is being used, SSD hard drives should be used. Refer to the column Standalone Server With GVFS for the recommended hardware settings.</t>
     </r>
   </si>
 </sst>
@@ -758,13 +928,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="72"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="20"/>
       <color rgb="FF006100"/>
@@ -796,8 +959,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -844,6 +1013,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="30">
     <border>
@@ -1181,9 +1362,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1301,7 +1482,6 @@
     <xf numFmtId="1" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1319,7 +1499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1334,6 +1514,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1458,7 +1686,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1475,12 +1703,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1488,7 +1710,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -1931,7 +2158,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -1953,44 +2180,44 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="77" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="75" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="79" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="80"/>
+      <c r="A5" s="90" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="94" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="95"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="75"/>
-      <c r="B6" s="50" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="51">
+      <c r="A6" s="90"/>
+      <c r="B6" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="50">
         <v>0</v>
       </c>
       <c r="D6" s="18" t="s">
@@ -1998,11 +2225,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="76"/>
-      <c r="B7" s="52" t="s">
+      <c r="A7" s="91"/>
+      <c r="B7" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="53">
+      <c r="C7" s="52">
         <v>0</v>
       </c>
       <c r="D7" s="18" t="s">
@@ -2023,7 +2250,7 @@
         <v>0.25</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2032,115 +2259,115 @@
       <c r="D10" s="18"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69" t="s">
+      <c r="D11" s="84"/>
+      <c r="E11" s="84"/>
+      <c r="F11" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69" t="s">
+      <c r="G11" s="84"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="69"/>
-      <c r="K11" s="70"/>
+      <c r="J11" s="84"/>
+      <c r="K11" s="85"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="78"/>
-      <c r="C12" s="71" t="s">
+      <c r="B12" s="93"/>
+      <c r="C12" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71" t="s">
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="71"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="71" t="s">
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="71"/>
-      <c r="K12" s="72"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="87"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="73" t="str">
+      <c r="C13" s="88" t="str">
         <f>IF(Current_Users&gt;STANDARD_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73" t="str">
+      <c r="D13" s="88"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="88" t="str">
         <f>IF(Current_Users&gt;HI_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73" t="str">
+      <c r="G13" s="88"/>
+      <c r="H13" s="88"/>
+      <c r="I13" s="88" t="str">
         <f>I14</f>
         <v>No</v>
       </c>
-      <c r="J13" s="73"/>
-      <c r="K13" s="74"/>
+      <c r="J13" s="88"/>
+      <c r="K13" s="89"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="73" t="str">
+      <c r="C14" s="88" t="str">
         <f>IF(Future_Users&gt;STANDARD_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73" t="str">
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88" t="str">
         <f>IF(Future_Users&gt;HI_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="73" t="str">
+      <c r="G14" s="88"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="88" t="str">
         <f>IF(Future_Users&gt;STANDARD_USERS,C_YES,C_NO)</f>
         <v>No</v>
       </c>
-      <c r="J14" s="73"/>
-      <c r="K14" s="74"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="89"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="73" t="str">
+      <c r="C15" s="88" t="str">
         <f>IF((COUNTIF(C13:C14,C_YES)&gt;1),C_YES,C_NO)</f>
         <v>Yes</v>
       </c>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73" t="str">
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="88" t="str">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;1),C_YES,C_NO)</f>
         <v>Yes</v>
       </c>
-      <c r="G15" s="73"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="73" t="str">
+      <c r="G15" s="88"/>
+      <c r="H15" s="88"/>
+      <c r="I15" s="88" t="str">
         <f>IF((COUNTIF(I13:I14,C_YES)&gt;0),C_YES,C_NO)</f>
         <v>No</v>
       </c>
-      <c r="J15" s="73"/>
-      <c r="K15" s="74"/>
+      <c r="J15" s="88"/>
+      <c r="K15" s="89"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="24" t="str">
         <f>IF(C13=C_YES,(IF(Current_Users&gt;LO_USERS,"Standard","Low-End")),"")</f>
@@ -2154,104 +2381,229 @@
         <f>IF(C14=C_YES,(IF(Future_Users&gt;LO_USERS,"Standard","Low-End")),"")</f>
         <v>Low-End</v>
       </c>
-      <c r="F16" s="63" t="str">
+      <c r="F16" s="78" t="str">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;0),"High-End","")</f>
         <v>High-End</v>
       </c>
-      <c r="G16" s="63"/>
-      <c r="H16" s="63"/>
-      <c r="I16" s="63" t="str">
+      <c r="G16" s="78"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="78" t="str">
         <f>IF((COUNTIF(I13:I14,C_YES)&gt;0),"Scale Unit","")</f>
         <v/>
       </c>
-      <c r="J16" s="63"/>
-      <c r="K16" s="64"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="79"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="65">
+        <v>36</v>
+      </c>
+      <c r="C17" s="80">
         <f>IF(C13=C_YES,(IF(Current_Users&gt;LO_USERS,STANDARD_TPC,LO_TPC)),"")</f>
         <v>5</v>
       </c>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65">
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="80">
         <f>IF(F13=C_YES,HIGH_TPC,"")</f>
         <v>75</v>
       </c>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65" t="str">
+      <c r="G17" s="80"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="80" t="str">
         <f>IF(I13=C_YES,SCALE_TPC,"")</f>
         <v/>
       </c>
-      <c r="J17" s="65"/>
-      <c r="K17" s="66"/>
+      <c r="J17" s="80"/>
+      <c r="K17" s="81"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="67">
+        <v>37</v>
+      </c>
+      <c r="C18" s="82">
         <f>IF(C13=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_TPC,LO_TPC)),"")</f>
         <v>5</v>
       </c>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="65">
+      <c r="D18" s="82"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="80">
         <f>IF(F14=C_YES,HIGH_TPC,"")</f>
         <v>75</v>
       </c>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="67" t="str">
+      <c r="G18" s="80"/>
+      <c r="H18" s="80"/>
+      <c r="I18" s="82" t="str">
         <f>IF(I14=C_YES,SCALE_TPC,"")</f>
         <v/>
       </c>
-      <c r="J18" s="67"/>
-      <c r="K18" s="68"/>
+      <c r="J18" s="82"/>
+      <c r="K18" s="83"/>
     </row>
     <row r="19" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="61">
+      <c r="B19" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="76">
         <f>IF((COUNTIF(C13:C14,C_YES)&gt;0),1,"")</f>
         <v>1</v>
       </c>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61">
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;0),1,"")</f>
         <v>1</v>
       </c>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="58" t="str">
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="57" t="str">
         <f>IF(I13=C_YES,ROUNDUP((Current_Users*SCALE_FACTOR)/SCALE_RPS,0),"")</f>
         <v/>
       </c>
-      <c r="J19" s="59" t="str">
+      <c r="J19" s="58" t="str">
         <f>IF(K19&lt;&gt;"","-","")</f>
         <v/>
       </c>
-      <c r="K19" s="60" t="str">
+      <c r="K19" s="59" t="str">
         <f>IF(I14=C_YES,ROUNDUP((Future_Users*HI_FACTOR)/SCALE_RPS,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="91.8" x14ac:dyDescent="1.65">
-      <c r="B22" s="49"/>
+    <row r="20" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="73" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="74"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="75"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="65"/>
+      <c r="K22" s="66"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="67"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="69"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="67"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="68"/>
+      <c r="J24" s="68"/>
+      <c r="K24" s="69"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="67"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="69"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="67"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="68"/>
+      <c r="K26" s="69"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="67"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="67"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="68"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="68"/>
+      <c r="J28" s="68"/>
+      <c r="K28" s="69"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="67"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="68"/>
+      <c r="J29" s="68"/>
+      <c r="K29" s="69"/>
+    </row>
+    <row r="30" spans="2:11" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="70"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="72"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="31">
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C17:E17"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="F12:H12"/>
@@ -2260,6 +2612,8 @@
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B22:K30"/>
+    <mergeCell ref="B21:K21"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="B2:K2"/>
@@ -2274,29 +2628,27 @@
     <mergeCell ref="I14:K14"/>
     <mergeCell ref="I15:K15"/>
     <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C17:E17"/>
   </mergeCells>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="19" priority="13">
+    <cfRule type="expression" dxfId="20" priority="13">
       <formula>$C$6&gt;=$C$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D8 D10">
-    <cfRule type="expression" dxfId="18" priority="12">
+    <cfRule type="expression" dxfId="19" priority="12">
       <formula>$C$7&lt;=$C$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:C15 F13:F16 I13:I16">
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="expression" dxfId="15" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>$C$9&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2353,39 +2705,39 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="14">
         <v>92</v>
@@ -2411,7 +2763,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="14">
         <v>180</v>
@@ -2437,7 +2789,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="14">
         <v>476</v>
@@ -2473,7 +2825,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="14">
         <v>730</v>
@@ -2508,7 +2860,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="14">
         <v>476</v>
@@ -2542,42 +2894,42 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="55" t="s">
-        <v>53</v>
+      <c r="A8" s="54" t="s">
+        <v>52</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" s="54">
+        <v>72</v>
+      </c>
+      <c r="B9" s="53">
         <v>250</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="53">
         <v>4</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="14">
         <v>500</v>
@@ -2589,12 +2941,12 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="14">
         <v>1000</v>
@@ -2606,18 +2958,18 @@
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="55" t="s">
-        <v>60</v>
+      <c r="A13" s="54" t="s">
+        <v>59</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>20</v>
@@ -2625,7 +2977,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="14">
         <v>450</v>
@@ -2639,7 +2991,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="14">
         <v>2200</v>
@@ -2653,7 +3005,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" s="14">
         <v>3600</v>
@@ -2670,40 +3022,40 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="29">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="56">
+        <v>61</v>
+      </c>
+      <c r="B19" s="55">
         <v>1.5</v>
       </c>
       <c r="D19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B20" s="29">
         <v>0.2</v>
       </c>
       <c r="D20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>21</v>
@@ -2724,9 +3076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:M33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2738,63 +3088,63 @@
   <sheetData>
     <row r="1" spans="2:13" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="73" t="str">
+      <c r="B2" s="88" t="str">
         <f>'Server Scenarios'!B2:K2</f>
         <v>Version 2019.04.21</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="81" t="s">
-        <v>47</v>
+      <c r="B6" s="96" t="s">
+        <v>46</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="94" t="s">
+      <c r="D6" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="95"/>
-      <c r="F6" s="94" t="s">
+      <c r="E6" s="110"/>
+      <c r="F6" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="96"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="96"/>
-      <c r="J6" s="94" t="s">
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="96"/>
-      <c r="L6" s="96"/>
-      <c r="M6" s="95"/>
+      <c r="K6" s="111"/>
+      <c r="L6" s="111"/>
+      <c r="M6" s="110"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="82"/>
+      <c r="B7" s="97"/>
       <c r="C7" s="3"/>
       <c r="D7" s="13" t="s">
         <v>13</v>
@@ -2802,25 +3152,25 @@
       <c r="E7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="97" t="s">
+      <c r="F7" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="98"/>
-      <c r="H7" s="99" t="s">
+      <c r="G7" s="113"/>
+      <c r="H7" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="98"/>
-      <c r="J7" s="97" t="s">
+      <c r="I7" s="113"/>
+      <c r="J7" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="98"/>
-      <c r="L7" s="99" t="s">
+      <c r="K7" s="113"/>
+      <c r="L7" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="100"/>
+      <c r="M7" s="115"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="82"/>
+      <c r="B8" s="97"/>
       <c r="C8" s="3"/>
       <c r="D8" s="13" t="s">
         <v>8</v>
@@ -2854,7 +3204,7 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="82"/>
+      <c r="B9" s="97"/>
       <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
@@ -2900,7 +3250,7 @@
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="82"/>
+      <c r="B10" s="97"/>
       <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
@@ -2946,7 +3296,7 @@
       </c>
     </row>
     <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="82"/>
+      <c r="B11" s="97"/>
       <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
@@ -2992,32 +3342,32 @@
       </c>
     </row>
     <row r="12" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="82"/>
+      <c r="B12" s="97"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="82"/>
+      <c r="B13" s="97"/>
       <c r="C13" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="87" t="s">
+      <c r="D13" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="88"/>
-      <c r="F13" s="87" t="s">
+      <c r="E13" s="103"/>
+      <c r="F13" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="89"/>
-      <c r="H13" s="89"/>
-      <c r="I13" s="89"/>
-      <c r="J13" s="87" t="s">
+      <c r="G13" s="104"/>
+      <c r="H13" s="104"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="89"/>
-      <c r="L13" s="89"/>
-      <c r="M13" s="88"/>
+      <c r="K13" s="104"/>
+      <c r="L13" s="104"/>
+      <c r="M13" s="103"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="82"/>
+      <c r="B14" s="97"/>
       <c r="C14" s="9"/>
       <c r="D14" s="41" t="s">
         <v>13</v>
@@ -3025,25 +3375,25 @@
       <c r="E14" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="90" t="s">
+      <c r="F14" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="91"/>
-      <c r="H14" s="92" t="s">
+      <c r="G14" s="106"/>
+      <c r="H14" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="91"/>
-      <c r="J14" s="90" t="s">
+      <c r="I14" s="106"/>
+      <c r="J14" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="91"/>
-      <c r="L14" s="92" t="s">
+      <c r="K14" s="106"/>
+      <c r="L14" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="93"/>
+      <c r="M14" s="108"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="82"/>
+      <c r="B15" s="97"/>
       <c r="C15" s="9"/>
       <c r="D15" s="41" t="s">
         <v>8</v>
@@ -3077,7 +3427,7 @@
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="82"/>
+      <c r="B16" s="97"/>
       <c r="C16" s="31" t="s">
         <v>17</v>
       </c>
@@ -3123,7 +3473,7 @@
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="82"/>
+      <c r="B17" s="97"/>
       <c r="C17" s="31" t="s">
         <v>20</v>
       </c>
@@ -3169,7 +3519,7 @@
       </c>
     </row>
     <row r="18" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="83"/>
+      <c r="B18" s="98"/>
       <c r="C18" s="32" t="s">
         <v>19</v>
       </c>
@@ -3216,31 +3566,31 @@
     </row>
     <row r="20" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="84" t="s">
-        <v>48</v>
+      <c r="B21" s="99" t="s">
+        <v>47</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="87" t="s">
+      <c r="D21" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="88"/>
-      <c r="F21" s="87" t="s">
+      <c r="E21" s="103"/>
+      <c r="F21" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="89"/>
-      <c r="H21" s="89"/>
-      <c r="I21" s="88"/>
-      <c r="J21" s="87" t="s">
+      <c r="G21" s="104"/>
+      <c r="H21" s="104"/>
+      <c r="I21" s="103"/>
+      <c r="J21" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="K21" s="89"/>
-      <c r="L21" s="89"/>
-      <c r="M21" s="88"/>
+      <c r="K21" s="104"/>
+      <c r="L21" s="104"/>
+      <c r="M21" s="103"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="85"/>
+      <c r="B22" s="100"/>
       <c r="C22" s="3"/>
       <c r="D22" s="41" t="s">
         <v>13</v>
@@ -3248,25 +3598,25 @@
       <c r="E22" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="90" t="s">
+      <c r="F22" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="91"/>
-      <c r="H22" s="92" t="s">
+      <c r="G22" s="106"/>
+      <c r="H22" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="93"/>
-      <c r="J22" s="90" t="s">
+      <c r="I22" s="108"/>
+      <c r="J22" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="91"/>
-      <c r="L22" s="92" t="s">
+      <c r="K22" s="106"/>
+      <c r="L22" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="M22" s="93"/>
+      <c r="M22" s="108"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="85"/>
+      <c r="B23" s="100"/>
       <c r="C23" s="3"/>
       <c r="D23" s="41" t="s">
         <v>8</v>
@@ -3300,7 +3650,7 @@
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="85"/>
+      <c r="B24" s="100"/>
       <c r="C24" s="4" t="s">
         <v>17</v>
       </c>
@@ -3346,7 +3696,7 @@
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="85"/>
+      <c r="B25" s="100"/>
       <c r="C25" s="4" t="s">
         <v>18</v>
       </c>
@@ -3392,7 +3742,7 @@
       </c>
     </row>
     <row r="26" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="85"/>
+      <c r="B26" s="100"/>
       <c r="C26" s="5" t="s">
         <v>19</v>
       </c>
@@ -3438,7 +3788,7 @@
       </c>
     </row>
     <row r="27" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="85"/>
+      <c r="B27" s="100"/>
       <c r="D27" s="46"/>
       <c r="E27" s="46"/>
       <c r="F27" s="46"/>
@@ -3451,29 +3801,29 @@
       <c r="M27" s="46"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="85"/>
+      <c r="B28" s="100"/>
       <c r="C28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="87" t="s">
+      <c r="D28" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="88"/>
-      <c r="F28" s="87" t="s">
+      <c r="E28" s="103"/>
+      <c r="F28" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="G28" s="89"/>
-      <c r="H28" s="89"/>
-      <c r="I28" s="88"/>
-      <c r="J28" s="87" t="s">
+      <c r="G28" s="104"/>
+      <c r="H28" s="104"/>
+      <c r="I28" s="103"/>
+      <c r="J28" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="K28" s="89"/>
-      <c r="L28" s="89"/>
-      <c r="M28" s="88"/>
+      <c r="K28" s="104"/>
+      <c r="L28" s="104"/>
+      <c r="M28" s="103"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B29" s="85"/>
+      <c r="B29" s="100"/>
       <c r="C29" s="3"/>
       <c r="D29" s="41" t="s">
         <v>13</v>
@@ -3481,25 +3831,25 @@
       <c r="E29" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="F29" s="90" t="s">
+      <c r="F29" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="91"/>
-      <c r="H29" s="92" t="s">
+      <c r="G29" s="106"/>
+      <c r="H29" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="I29" s="93"/>
-      <c r="J29" s="90" t="s">
+      <c r="I29" s="108"/>
+      <c r="J29" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="K29" s="91"/>
-      <c r="L29" s="92" t="s">
+      <c r="K29" s="106"/>
+      <c r="L29" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="M29" s="93"/>
+      <c r="M29" s="108"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="85"/>
+      <c r="B30" s="100"/>
       <c r="C30" s="3"/>
       <c r="D30" s="41" t="s">
         <v>8</v>
@@ -3533,7 +3883,7 @@
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="85"/>
+      <c r="B31" s="100"/>
       <c r="C31" s="4" t="s">
         <v>17</v>
       </c>
@@ -3579,7 +3929,7 @@
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B32" s="85"/>
+      <c r="B32" s="100"/>
       <c r="C32" s="4" t="s">
         <v>20</v>
       </c>
@@ -3625,7 +3975,7 @@
       </c>
     </row>
     <row r="33" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="86"/>
+      <c r="B33" s="101"/>
       <c r="C33" s="5" t="s">
         <v>19</v>
       </c>
@@ -3706,7 +4056,7 @@
     <mergeCell ref="J22:K22"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:M33">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3717,7 +4067,578 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B24151-BCDB-4D54-B778-984CD476EECE}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:K32"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" customWidth="1"/>
+    <col min="9" max="10" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="88" t="str">
+        <f>'Server Scenarios'!B2:K2</f>
+        <v>Version 2019.04.21</v>
+      </c>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="90" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="120" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="121"/>
+      <c r="D6" s="131" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="120" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="121"/>
+      <c r="H6" s="120" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="121"/>
+    </row>
+    <row r="7" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="90"/>
+      <c r="B7" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="50">
+        <v>0</v>
+      </c>
+      <c r="D7" s="131"/>
+      <c r="E7" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="50">
+        <v>0</v>
+      </c>
+      <c r="H7" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="63">
+        <f>Future_Users</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="91"/>
+      <c r="B8" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="52">
+        <v>0</v>
+      </c>
+      <c r="D8" s="131"/>
+      <c r="E8" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="52">
+        <v>0</v>
+      </c>
+      <c r="H8" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="62">
+        <f>Current_Users</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="119" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="128" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="129"/>
+      <c r="E11" s="129"/>
+      <c r="F11" s="130"/>
+      <c r="G11" s="109" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="110"/>
+      <c r="I11" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" s="110"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="97"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="117"/>
+      <c r="E12" s="117"/>
+      <c r="F12" s="118"/>
+      <c r="G12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="97"/>
+      <c r="C13" s="122" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="123"/>
+      <c r="E13" s="123"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="33">
+        <f>IF(Current_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Current_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="35">
+        <f>G13*(1+VM_OVERHEAD)</f>
+        <v>1.2</v>
+      </c>
+      <c r="I13" s="33">
+        <f>IF(Current_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Current_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
+        <v>1</v>
+      </c>
+      <c r="J13" s="35">
+        <f>I13*(1+VM_OVERHEAD)</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="97"/>
+      <c r="C14" s="122" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="123"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="33">
+        <f>IF(Current_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_RAM, IF(Current_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_RAM,PROXY_MEDIUM_RAM))</f>
+        <v>2</v>
+      </c>
+      <c r="H14" s="35">
+        <f>G14*(1+VM_OVERHEAD)</f>
+        <v>2.4</v>
+      </c>
+      <c r="I14" s="33">
+        <f>G14+(Current_BranchTip)</f>
+        <v>2</v>
+      </c>
+      <c r="J14" s="35">
+        <f>I14*(1+VM_OVERHEAD)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="97"/>
+      <c r="C15" s="125" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="126"/>
+      <c r="E15" s="126"/>
+      <c r="F15" s="127"/>
+      <c r="G15" s="34">
+        <f>Current_BranchTip</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="47">
+        <f>G15</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="34">
+        <f>Current_Storage*GVFS_SCALE_FACTOR</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="47">
+        <f>I15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="97"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="97"/>
+      <c r="C17" s="128" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="129"/>
+      <c r="E17" s="129"/>
+      <c r="F17" s="130"/>
+      <c r="G17" s="109" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="110"/>
+      <c r="I17" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="110"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="97"/>
+      <c r="C18" s="116"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="118"/>
+      <c r="G18" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" s="42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="97"/>
+      <c r="C19" s="122" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="123"/>
+      <c r="E19" s="123"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="33">
+        <f>IF(Future_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Future_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="35">
+        <f>G19*(1+VM_OVERHEAD)</f>
+        <v>1.2</v>
+      </c>
+      <c r="I19" s="33">
+        <f>IF(Future_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Future_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
+        <v>1</v>
+      </c>
+      <c r="J19" s="35">
+        <f>I19*(1+VM_OVERHEAD)</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="97"/>
+      <c r="C20" s="122" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="123"/>
+      <c r="E20" s="123"/>
+      <c r="F20" s="124"/>
+      <c r="G20" s="33">
+        <f>IF(Future_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_RAM, IF(Future_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_RAM,PROXY_MEDIUM_RAM))</f>
+        <v>2</v>
+      </c>
+      <c r="H20" s="35">
+        <f>G20*(1+VM_OVERHEAD)</f>
+        <v>2.4</v>
+      </c>
+      <c r="I20" s="33">
+        <f>G20+Future_BranchTip</f>
+        <v>2</v>
+      </c>
+      <c r="J20" s="35">
+        <f>I20*(1+VM_OVERHEAD)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="98"/>
+      <c r="C21" s="125" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="126"/>
+      <c r="E21" s="126"/>
+      <c r="F21" s="127"/>
+      <c r="G21" s="34">
+        <f>Future_BranchTip</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="47">
+        <f>G21</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="34">
+        <f>Future_Storage*GVFS_SCALE_FACTOR</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="47">
+        <f>I21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="73" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="75"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="66"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="67"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="69"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="67"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="68"/>
+      <c r="K26" s="69"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="67"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="67"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="68"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="68"/>
+      <c r="J28" s="68"/>
+      <c r="K28" s="69"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="67"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="68"/>
+      <c r="J29" s="68"/>
+      <c r="K29" s="69"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="67"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="68"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="68"/>
+      <c r="H30" s="68"/>
+      <c r="I30" s="68"/>
+      <c r="J30" s="68"/>
+      <c r="K30" s="69"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B31" s="67"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="68"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="68"/>
+      <c r="H31" s="68"/>
+      <c r="I31" s="68"/>
+      <c r="J31" s="68"/>
+      <c r="K31" s="69"/>
+    </row>
+    <row r="32" spans="2:11" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="70"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="71"/>
+      <c r="K32" s="72"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="23">
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="B23:K23"/>
+    <mergeCell ref="B24:K32"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B11:B21"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C21:F21"/>
+  </mergeCells>
+  <conditionalFormatting sqref="G10:H10">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18:H21 G12:H16">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:H11">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17:H17">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12:J12 J13:J15">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11:J11">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18:J18 J19:J21">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19:I21">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17:J17">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13:I15">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>Current_Storage&lt;=Future_Storage</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>Current_BranchTip &lt;= Future_BranchTip</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9C01BD-A0E7-4C75-963D-65D4B351A825}">
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
@@ -3737,607 +4658,362 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="73" t="str">
+      <c r="B2" s="88" t="str">
         <f>'Server Scenarios'!B2:K2</f>
         <v>Version 2019.04.21</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="75" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="105" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="106"/>
-      <c r="D7" s="116" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="105" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="106"/>
-      <c r="H7" s="105" t="s">
+      <c r="A7" s="90" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="120" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="121"/>
+      <c r="E7" s="120" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="121"/>
+    </row>
+    <row r="8" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="90"/>
+      <c r="B8" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="50">
+        <v>0</v>
+      </c>
+      <c r="E8" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="I7" s="106"/>
-    </row>
-    <row r="8" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="75"/>
-      <c r="B8" s="50" t="s">
+      <c r="F8" s="63">
+        <f>Future_Users</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="91"/>
+      <c r="B9" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="51">
-        <v>0</v>
-      </c>
-      <c r="D8" s="116"/>
-      <c r="E8" s="50" t="s">
+      <c r="C9" s="52">
+        <v>0</v>
+      </c>
+      <c r="E9" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="51">
-        <v>0</v>
-      </c>
-      <c r="H8" s="50" t="s">
-        <v>78</v>
-      </c>
-      <c r="I8" s="118">
-        <f>Future_Users</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="76"/>
-      <c r="B9" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="53">
-        <v>0</v>
-      </c>
-      <c r="D9" s="116"/>
-      <c r="E9" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="51">
-        <v>0</v>
-      </c>
-      <c r="H9" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="117">
+      <c r="F9" s="62">
         <f>Current_Users</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E10" s="52" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="119" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="128" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="129"/>
+      <c r="E12" s="129"/>
+      <c r="F12" s="130"/>
+      <c r="G12" s="109" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="110"/>
+    </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="104" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="113" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="114"/>
-      <c r="E13" s="114"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="94" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="95"/>
+      <c r="B13" s="97"/>
+      <c r="C13" s="116"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="118"/>
+      <c r="G13" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="82"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="102"/>
-      <c r="E14" s="102"/>
-      <c r="F14" s="103"/>
-      <c r="G14" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="82"/>
-      <c r="C15" s="107" t="s">
+      <c r="B14" s="97"/>
+      <c r="C14" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="108"/>
-      <c r="E15" s="108"/>
-      <c r="F15" s="109"/>
-      <c r="G15" s="33">
+      <c r="D14" s="123"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="33">
         <f>IF(Current_Users&gt;CS_LOW_USERS,CS_HIGH_CORES,CS_LOW_CORES)</f>
         <v>2</v>
       </c>
+      <c r="H14" s="35">
+        <f>G14*(1+VM_OVERHEAD)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="97"/>
+      <c r="C15" s="122" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="123"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="33">
+        <f>IF(Current_Users&gt;CS_LOW_USERS,CS_HIGH_RAM,CS_LOW_RAM)</f>
+        <v>8</v>
+      </c>
       <c r="H15" s="35">
         <f>G15*(1+VM_OVERHEAD)</f>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="82"/>
-      <c r="C16" s="107" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="108"/>
-      <c r="E16" s="108"/>
-      <c r="F16" s="109"/>
-      <c r="G16" s="33">
-        <f>IF(Current_Users&gt;CS_LOW_USERS,CS_HIGH_RAM,CS_LOW_RAM)</f>
-        <v>8</v>
-      </c>
-      <c r="H16" s="35">
-        <f>G16*(1+VM_OVERHEAD)</f>
         <v>9.6</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="82"/>
-      <c r="C17" s="110" t="s">
+    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="97"/>
+      <c r="C16" s="125" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="111"/>
-      <c r="E17" s="111"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="34">
+      <c r="D16" s="126"/>
+      <c r="E16" s="126"/>
+      <c r="F16" s="127"/>
+      <c r="G16" s="34">
         <f>Current_Storage*CS_STORAGE_FACTOR</f>
         <v>0</v>
       </c>
-      <c r="H17" s="47">
-        <f>G17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="82"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="82"/>
-      <c r="C19" s="113" t="s">
+      <c r="H16" s="47">
+        <f>G16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="97"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="97"/>
+      <c r="C18" s="128" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="114"/>
-      <c r="E19" s="114"/>
-      <c r="F19" s="115"/>
-      <c r="G19" s="94" t="s">
-        <v>54</v>
-      </c>
-      <c r="H19" s="95"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="82"/>
-      <c r="C20" s="101"/>
-      <c r="D20" s="102"/>
-      <c r="E20" s="102"/>
-      <c r="F20" s="103"/>
-      <c r="G20" s="41" t="s">
+      <c r="D18" s="129"/>
+      <c r="E18" s="129"/>
+      <c r="F18" s="130"/>
+      <c r="G18" s="109" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="110"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="97"/>
+      <c r="C19" s="116"/>
+      <c r="D19" s="117"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="118"/>
+      <c r="G19" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="42" t="s">
+      <c r="H19" s="42" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="82"/>
-      <c r="C21" s="107" t="s">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="97"/>
+      <c r="C20" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="108"/>
-      <c r="E21" s="108"/>
-      <c r="F21" s="109"/>
-      <c r="G21" s="33">
+      <c r="D20" s="123"/>
+      <c r="E20" s="123"/>
+      <c r="F20" s="124"/>
+      <c r="G20" s="33">
         <f>IF(Future_Users&gt;CS_LOW_USERS,CS_HIGH_CORES,CS_LOW_CORES)</f>
         <v>2</v>
       </c>
+      <c r="H20" s="35">
+        <f>G20*(1+VM_OVERHEAD)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="97"/>
+      <c r="C21" s="122" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="123"/>
+      <c r="E21" s="123"/>
+      <c r="F21" s="124"/>
+      <c r="G21" s="33">
+        <f>IF(Future_Users&gt;CS_LOW_USERS,CS_HIGH_RAM,CS_LOW_RAM)</f>
+        <v>8</v>
+      </c>
       <c r="H21" s="35">
         <f>G21*(1+VM_OVERHEAD)</f>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="82"/>
-      <c r="C22" s="107" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="108"/>
-      <c r="E22" s="108"/>
-      <c r="F22" s="109"/>
-      <c r="G22" s="33">
-        <f>IF(Future_Users&gt;CS_LOW_USERS,CS_HIGH_RAM,CS_LOW_RAM)</f>
-        <v>8</v>
-      </c>
-      <c r="H22" s="35">
-        <f>G22*(1+VM_OVERHEAD)</f>
         <v>9.6</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="83"/>
-      <c r="C23" s="110" t="s">
+    <row r="22" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="98"/>
+      <c r="C22" s="125" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="111"/>
-      <c r="E23" s="111"/>
-      <c r="F23" s="112"/>
-      <c r="G23" s="34">
+      <c r="D22" s="126"/>
+      <c r="E22" s="126"/>
+      <c r="F22" s="127"/>
+      <c r="G22" s="34">
         <f>Future_Storage*CS_STORAGE_FACTOR</f>
         <v>0</v>
       </c>
-      <c r="H23" s="47">
-        <f>G23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B25" s="104" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="113" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="114"/>
-      <c r="E25" s="114"/>
-      <c r="F25" s="115"/>
-      <c r="G25" s="94" t="s">
-        <v>54</v>
-      </c>
-      <c r="H25" s="95"/>
-      <c r="I25" s="94" t="s">
-        <v>61</v>
-      </c>
-      <c r="J25" s="95"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B26" s="82"/>
-      <c r="C26" s="101"/>
-      <c r="D26" s="102"/>
-      <c r="E26" s="102"/>
-      <c r="F26" s="103"/>
-      <c r="G26" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I26" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="J26" s="42" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="82"/>
-      <c r="C27" s="107" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="108"/>
-      <c r="E27" s="108"/>
-      <c r="F27" s="109"/>
-      <c r="G27" s="33">
-        <f>IF(Current_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Current_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
-        <v>1</v>
-      </c>
-      <c r="H27" s="35">
-        <f>G27*(1+VM_OVERHEAD)</f>
-        <v>1.2</v>
-      </c>
-      <c r="I27" s="33">
-        <f>IF(Current_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Current_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
-        <v>1</v>
-      </c>
-      <c r="J27" s="35">
-        <f>I27*(1+VM_OVERHEAD)</f>
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="82"/>
-      <c r="C28" s="107" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="108"/>
-      <c r="E28" s="108"/>
-      <c r="F28" s="109"/>
-      <c r="G28" s="33">
-        <f>IF(Current_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_RAM, IF(Current_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_RAM,PROXY_MEDIUM_RAM))</f>
-        <v>2</v>
-      </c>
-      <c r="H28" s="35">
-        <f>G28*(1+VM_OVERHEAD)</f>
-        <v>2.4</v>
-      </c>
-      <c r="I28" s="33">
-        <f>G28+(Current_BranchTip)</f>
-        <v>2</v>
-      </c>
-      <c r="J28" s="35">
-        <f>I28*(1+VM_OVERHEAD)</f>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="82"/>
-      <c r="C29" s="110" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="111"/>
-      <c r="E29" s="111"/>
-      <c r="F29" s="112"/>
-      <c r="G29" s="34">
-        <f>Current_BranchTip*Active_Branches</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="47">
-        <f>G29</f>
-        <v>0</v>
-      </c>
-      <c r="I29" s="34">
-        <f>Current_Storage*GVFS_SCALE_FACTOR</f>
-        <v>0</v>
-      </c>
-      <c r="J29" s="47">
-        <f>I29</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="82"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B31" s="82"/>
-      <c r="C31" s="113" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="114"/>
-      <c r="E31" s="114"/>
-      <c r="F31" s="115"/>
-      <c r="G31" s="94" t="s">
-        <v>54</v>
-      </c>
-      <c r="H31" s="95"/>
-      <c r="I31" s="94" t="s">
-        <v>61</v>
-      </c>
-      <c r="J31" s="95"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B32" s="82"/>
-      <c r="C32" s="101"/>
-      <c r="D32" s="102"/>
-      <c r="E32" s="102"/>
-      <c r="F32" s="103"/>
-      <c r="G32" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="H32" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="I32" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="J32" s="42" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B33" s="82"/>
-      <c r="C33" s="107" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" s="108"/>
-      <c r="E33" s="108"/>
-      <c r="F33" s="109"/>
-      <c r="G33" s="33">
-        <f>IF(Future_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Future_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
-        <v>1</v>
-      </c>
-      <c r="H33" s="35">
-        <f>G33*(1+VM_OVERHEAD)</f>
-        <v>1.2</v>
-      </c>
-      <c r="I33" s="33">
-        <f>IF(Future_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Future_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
-        <v>1</v>
-      </c>
-      <c r="J33" s="35">
-        <f>I33*(1+VM_OVERHEAD)</f>
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B34" s="82"/>
-      <c r="C34" s="107" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="108"/>
-      <c r="E34" s="108"/>
-      <c r="F34" s="109"/>
-      <c r="G34" s="33">
-        <f>IF(Future_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_RAM, IF(Future_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_RAM,PROXY_MEDIUM_RAM))</f>
-        <v>2</v>
-      </c>
-      <c r="H34" s="35">
-        <f>G34*(1+VM_OVERHEAD)</f>
-        <v>2.4</v>
-      </c>
-      <c r="I34" s="33">
-        <f>G34+Future_BranchTip</f>
-        <v>2</v>
-      </c>
-      <c r="J34" s="35">
-        <f>I34*(1+VM_OVERHEAD)</f>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="83"/>
-      <c r="C35" s="110" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" s="111"/>
-      <c r="E35" s="111"/>
-      <c r="F35" s="112"/>
-      <c r="G35" s="34">
-        <f>Future_BranchTip*Active_Branches</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="47">
-        <f>G35</f>
-        <v>0</v>
-      </c>
-      <c r="I35" s="34">
-        <f>Future_Storage*GVFS_SCALE_FACTOR</f>
-        <v>0</v>
-      </c>
-      <c r="J35" s="47">
-        <f>I35</f>
-        <v>0</v>
-      </c>
+      <c r="H22" s="47">
+        <f>G22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="73" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="74"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="74"/>
+      <c r="K24" s="75"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="64" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="65"/>
+      <c r="K25" s="66"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="67"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="68"/>
+      <c r="K26" s="69"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="67"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="67"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="68"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="68"/>
+      <c r="J28" s="68"/>
+      <c r="K28" s="69"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="67"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="68"/>
+      <c r="J29" s="68"/>
+      <c r="K29" s="69"/>
+    </row>
+    <row r="30" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="70"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="72"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="34">
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="H7:I7"/>
+  <mergeCells count="19">
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="B24:K24"/>
+    <mergeCell ref="B25:K30"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="B12:B22"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C14:F14"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="G18:H18"/>
     <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B25:B35"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C29:F29"/>
   </mergeCells>
-  <conditionalFormatting sqref="G13:H24">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+  <conditionalFormatting sqref="G12:H23">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
       <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G32:H35 G26:H30">
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G25:H25">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G31:H31">
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I26:J26 J27:J29">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I25:J25">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32:J32 J33:J35">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33:I35">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31:J31">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I27:I29">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>Current_Storage&lt;=Future_Storage</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>Current_BranchTip &lt;= Future_BranchTip</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4457,11 +5133,11 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{312B28CD-EB51-4560-8E58-B9E03DAFD80D}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="d4f1fd26-cd3f-48df-8559-6269d85163e3"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>

</xml_diff>

<commit_message>
Add instructions to spreadsheets (#73)
</commit_message>
<xml_diff>
--- a/src/Planning/understand-options-azure-devops-environments-capacity-guide.xlsx
+++ b/src/Planning/understand-options-azure-devops-environments-capacity-guide.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ken.muse\Source\Repos\ALMRangers Guidance\src\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ken.muse\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988E16C4-3487-44E7-BFF3-7C4BB7FE4FFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{91AF45C8-2D9E-4696-8D1D-8977D2C692C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,10 +16,10 @@
     <sheet name="Server Scenarios" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="5" state="hidden" r:id="rId2"/>
     <sheet name="Hardware Configurations" sheetId="7" r:id="rId3"/>
-    <sheet name="Additional Servers" sheetId="8" r:id="rId4"/>
+    <sheet name="Proxy Server" sheetId="8" r:id="rId4"/>
+    <sheet name="Code Search Server" sheetId="9" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="Active_Branches">'Additional Servers'!$F$10</definedName>
     <definedName name="BEEF_FACTOR">'Server Scenarios'!$C$9</definedName>
     <definedName name="C_NO">Constants!$B$22</definedName>
     <definedName name="C_YES">Constants!$B$21</definedName>
@@ -33,13 +33,15 @@
     <definedName name="CS_LOW_RAM">Constants!$D$10</definedName>
     <definedName name="CS_LOW_USERS">Constants!$B$10</definedName>
     <definedName name="CS_STORAGE_FACTOR">Constants!$B$19</definedName>
-    <definedName name="Current_BranchTip">'Additional Servers'!$F$9</definedName>
-    <definedName name="Current_Storage">'Additional Servers'!$C$9</definedName>
+    <definedName name="Current_BranchTip">'Proxy Server'!$F$8</definedName>
+    <definedName name="Current_Storage" localSheetId="4">'Code Search Server'!$C$9</definedName>
+    <definedName name="Current_Storage">'Proxy Server'!$C$8</definedName>
     <definedName name="Current_Users">'Server Scenarios'!$C$7</definedName>
     <definedName name="DUAL_CURRENT_OK">'Server Scenarios'!$F$13</definedName>
     <definedName name="DUAL_FUTURE_OK">'Server Scenarios'!$F$14</definedName>
-    <definedName name="Future_BranchTip">'Additional Servers'!$F$8</definedName>
-    <definedName name="Future_Storage">'Additional Servers'!$C$8</definedName>
+    <definedName name="Future_BranchTip">'Proxy Server'!$F$7</definedName>
+    <definedName name="Future_Storage" localSheetId="4">'Code Search Server'!$C$8</definedName>
+    <definedName name="Future_Storage">'Proxy Server'!$C$7</definedName>
     <definedName name="Future_Users">'Server Scenarios'!$C$6</definedName>
     <definedName name="GVFS_SCALE_FACTOR">Constants!$B$18</definedName>
     <definedName name="HI_CORE_AT">Constants!$F$5</definedName>
@@ -114,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="91">
   <si>
     <t>F</t>
   </si>
@@ -277,9 +279,6 @@
     </r>
   </si>
   <si>
-    <t>NUMBER OF ACTIVE TEAM FOUNDATION SERVER USERS</t>
-  </si>
-  <si>
     <t>Low-End Configuration</t>
   </si>
   <si>
@@ -535,9 +534,6 @@
     <t>Maximum Expected</t>
   </si>
   <si>
-    <t>Active Branches</t>
-  </si>
-  <si>
     <t>Virtualization Overhead</t>
   </si>
   <si>
@@ -618,6 +614,180 @@
         <scheme val="minor"/>
       </rPr>
       <t>https://docs.microsoft.com/en-us/azure/devops/project/search/administration</t>
+    </r>
+  </si>
+  <si>
+    <t>INSTRUCTIONS</t>
+  </si>
+  <si>
+    <t>NUMBER OF ACTIVE AZURE DEVOPS SERVER USERS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To use this simplified capacity planning tool, enter the maximum number of users expected to be actively using the Azure DevOps servers. Then, enter the current number of users for the system. The Infrastructure Architecture table will automatically update to indicate suggested server configurations. The tab </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hardware Configurations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> will contain the suggested minimum hardware specifications for the servers.
+If the one or more teams will be operating remotely and using Team Foundation Version Control (TFVC) or Git Virtual File System (GVFS), then consider using an Azure DevOps Proxy server to improve the performance. This can be configured using the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Proxy Server</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tab.
+To enable full-text search across Code, Wiki, packages, and work items, a Code Search Server will be required. This can be configured on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Code Search</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tab.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To estimate the requirements for the Code Search Server, enter the current and maximum expected repository size. The hardware requirements will be reflected in the table above.  If you're working with a Git repository, you can estimate the size by issuing the following commands and reviewing the value of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>size-pack</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>git gc
+git count-objects -vH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To estimate the required configuration for the Proxy Server, enter the current and expected maximum size of all code repositories which will be accessed. If you're working with a Git repository, you can estimate the size by issuing the following commands and reviewing the value of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>size-pack</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">git gc
+git count-objects -vH
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Additionally, enter the current and expected maximum tip sizes for all active branches. This is the size of the files in each active branch as queried from the file system.
+If the Git Virtual File System (GVFS) proxy feature is being used, SSD hard drives should be used. Refer to the column Standalone Server With GVFS for the recommended hardware settings.</t>
     </r>
   </si>
 </sst>
@@ -758,13 +928,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="72"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="20"/>
       <color rgb="FF006100"/>
@@ -796,8 +959,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -844,6 +1013,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="30">
     <border>
@@ -1181,9 +1362,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1301,7 +1482,6 @@
     <xf numFmtId="1" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1319,7 +1499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1334,6 +1514,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1458,7 +1686,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1475,12 +1703,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1488,7 +1710,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -1931,7 +2158,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -1953,44 +2180,44 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="77" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="75" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="79" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="80"/>
+      <c r="A5" s="90" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="94" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="95"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="75"/>
-      <c r="B6" s="50" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="51">
+      <c r="A6" s="90"/>
+      <c r="B6" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="50">
         <v>0</v>
       </c>
       <c r="D6" s="18" t="s">
@@ -1998,11 +2225,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="76"/>
-      <c r="B7" s="52" t="s">
+      <c r="A7" s="91"/>
+      <c r="B7" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="53">
+      <c r="C7" s="52">
         <v>0</v>
       </c>
       <c r="D7" s="18" t="s">
@@ -2023,7 +2250,7 @@
         <v>0.25</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2032,115 +2259,115 @@
       <c r="D10" s="18"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69" t="s">
+      <c r="D11" s="84"/>
+      <c r="E11" s="84"/>
+      <c r="F11" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69" t="s">
+      <c r="G11" s="84"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="69"/>
-      <c r="K11" s="70"/>
+      <c r="J11" s="84"/>
+      <c r="K11" s="85"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="78"/>
-      <c r="C12" s="71" t="s">
+      <c r="B12" s="93"/>
+      <c r="C12" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71" t="s">
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="71"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="71" t="s">
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="71"/>
-      <c r="K12" s="72"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="87"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="73" t="str">
+      <c r="C13" s="88" t="str">
         <f>IF(Current_Users&gt;STANDARD_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73" t="str">
+      <c r="D13" s="88"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="88" t="str">
         <f>IF(Current_Users&gt;HI_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73" t="str">
+      <c r="G13" s="88"/>
+      <c r="H13" s="88"/>
+      <c r="I13" s="88" t="str">
         <f>I14</f>
         <v>No</v>
       </c>
-      <c r="J13" s="73"/>
-      <c r="K13" s="74"/>
+      <c r="J13" s="88"/>
+      <c r="K13" s="89"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="73" t="str">
+      <c r="C14" s="88" t="str">
         <f>IF(Future_Users&gt;STANDARD_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73" t="str">
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88" t="str">
         <f>IF(Future_Users&gt;HI_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="73" t="str">
+      <c r="G14" s="88"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="88" t="str">
         <f>IF(Future_Users&gt;STANDARD_USERS,C_YES,C_NO)</f>
         <v>No</v>
       </c>
-      <c r="J14" s="73"/>
-      <c r="K14" s="74"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="89"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="73" t="str">
+      <c r="C15" s="88" t="str">
         <f>IF((COUNTIF(C13:C14,C_YES)&gt;1),C_YES,C_NO)</f>
         <v>Yes</v>
       </c>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73" t="str">
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="88" t="str">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;1),C_YES,C_NO)</f>
         <v>Yes</v>
       </c>
-      <c r="G15" s="73"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="73" t="str">
+      <c r="G15" s="88"/>
+      <c r="H15" s="88"/>
+      <c r="I15" s="88" t="str">
         <f>IF((COUNTIF(I13:I14,C_YES)&gt;0),C_YES,C_NO)</f>
         <v>No</v>
       </c>
-      <c r="J15" s="73"/>
-      <c r="K15" s="74"/>
+      <c r="J15" s="88"/>
+      <c r="K15" s="89"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="24" t="str">
         <f>IF(C13=C_YES,(IF(Current_Users&gt;LO_USERS,"Standard","Low-End")),"")</f>
@@ -2154,104 +2381,229 @@
         <f>IF(C14=C_YES,(IF(Future_Users&gt;LO_USERS,"Standard","Low-End")),"")</f>
         <v>Low-End</v>
       </c>
-      <c r="F16" s="63" t="str">
+      <c r="F16" s="78" t="str">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;0),"High-End","")</f>
         <v>High-End</v>
       </c>
-      <c r="G16" s="63"/>
-      <c r="H16" s="63"/>
-      <c r="I16" s="63" t="str">
+      <c r="G16" s="78"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="78" t="str">
         <f>IF((COUNTIF(I13:I14,C_YES)&gt;0),"Scale Unit","")</f>
         <v/>
       </c>
-      <c r="J16" s="63"/>
-      <c r="K16" s="64"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="79"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="65">
+        <v>36</v>
+      </c>
+      <c r="C17" s="80">
         <f>IF(C13=C_YES,(IF(Current_Users&gt;LO_USERS,STANDARD_TPC,LO_TPC)),"")</f>
         <v>5</v>
       </c>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65">
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="80">
         <f>IF(F13=C_YES,HIGH_TPC,"")</f>
         <v>75</v>
       </c>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65" t="str">
+      <c r="G17" s="80"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="80" t="str">
         <f>IF(I13=C_YES,SCALE_TPC,"")</f>
         <v/>
       </c>
-      <c r="J17" s="65"/>
-      <c r="K17" s="66"/>
+      <c r="J17" s="80"/>
+      <c r="K17" s="81"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="67">
+        <v>37</v>
+      </c>
+      <c r="C18" s="82">
         <f>IF(C13=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_TPC,LO_TPC)),"")</f>
         <v>5</v>
       </c>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="65">
+      <c r="D18" s="82"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="80">
         <f>IF(F14=C_YES,HIGH_TPC,"")</f>
         <v>75</v>
       </c>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="67" t="str">
+      <c r="G18" s="80"/>
+      <c r="H18" s="80"/>
+      <c r="I18" s="82" t="str">
         <f>IF(I14=C_YES,SCALE_TPC,"")</f>
         <v/>
       </c>
-      <c r="J18" s="67"/>
-      <c r="K18" s="68"/>
+      <c r="J18" s="82"/>
+      <c r="K18" s="83"/>
     </row>
     <row r="19" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="61">
+      <c r="B19" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="76">
         <f>IF((COUNTIF(C13:C14,C_YES)&gt;0),1,"")</f>
         <v>1</v>
       </c>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61">
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;0),1,"")</f>
         <v>1</v>
       </c>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="58" t="str">
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="57" t="str">
         <f>IF(I13=C_YES,ROUNDUP((Current_Users*SCALE_FACTOR)/SCALE_RPS,0),"")</f>
         <v/>
       </c>
-      <c r="J19" s="59" t="str">
+      <c r="J19" s="58" t="str">
         <f>IF(K19&lt;&gt;"","-","")</f>
         <v/>
       </c>
-      <c r="K19" s="60" t="str">
+      <c r="K19" s="59" t="str">
         <f>IF(I14=C_YES,ROUNDUP((Future_Users*HI_FACTOR)/SCALE_RPS,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="91.8" x14ac:dyDescent="1.65">
-      <c r="B22" s="49"/>
+    <row r="20" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="73" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="74"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="75"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="65"/>
+      <c r="K22" s="66"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="67"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="69"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="67"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="68"/>
+      <c r="J24" s="68"/>
+      <c r="K24" s="69"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="67"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="69"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="67"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="68"/>
+      <c r="K26" s="69"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="67"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="67"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="68"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="68"/>
+      <c r="J28" s="68"/>
+      <c r="K28" s="69"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="67"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="68"/>
+      <c r="J29" s="68"/>
+      <c r="K29" s="69"/>
+    </row>
+    <row r="30" spans="2:11" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="70"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="72"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="31">
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C17:E17"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="F12:H12"/>
@@ -2260,6 +2612,8 @@
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B22:K30"/>
+    <mergeCell ref="B21:K21"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="B2:K2"/>
@@ -2274,29 +2628,27 @@
     <mergeCell ref="I14:K14"/>
     <mergeCell ref="I15:K15"/>
     <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C17:E17"/>
   </mergeCells>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="19" priority="13">
+    <cfRule type="expression" dxfId="20" priority="13">
       <formula>$C$6&gt;=$C$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D8 D10">
-    <cfRule type="expression" dxfId="18" priority="12">
+    <cfRule type="expression" dxfId="19" priority="12">
       <formula>$C$7&lt;=$C$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:C15 F13:F16 I13:I16">
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="expression" dxfId="15" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>$C$9&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2353,39 +2705,39 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="14">
         <v>92</v>
@@ -2411,7 +2763,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="14">
         <v>180</v>
@@ -2437,7 +2789,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="14">
         <v>476</v>
@@ -2473,7 +2825,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="14">
         <v>730</v>
@@ -2508,7 +2860,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="14">
         <v>476</v>
@@ -2542,42 +2894,42 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="55" t="s">
-        <v>53</v>
+      <c r="A8" s="54" t="s">
+        <v>52</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" s="54">
+        <v>72</v>
+      </c>
+      <c r="B9" s="53">
         <v>250</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="53">
         <v>4</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="14">
         <v>500</v>
@@ -2589,12 +2941,12 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="14">
         <v>1000</v>
@@ -2606,18 +2958,18 @@
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="55" t="s">
-        <v>60</v>
+      <c r="A13" s="54" t="s">
+        <v>59</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>20</v>
@@ -2625,7 +2977,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="14">
         <v>450</v>
@@ -2639,7 +2991,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="14">
         <v>2200</v>
@@ -2653,7 +3005,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" s="14">
         <v>3600</v>
@@ -2670,40 +3022,40 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="29">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="56">
+        <v>61</v>
+      </c>
+      <c r="B19" s="55">
         <v>1.5</v>
       </c>
       <c r="D19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B20" s="29">
         <v>0.2</v>
       </c>
       <c r="D20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>21</v>
@@ -2724,9 +3076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:M33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2738,63 +3088,63 @@
   <sheetData>
     <row r="1" spans="2:13" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="73" t="str">
+      <c r="B2" s="88" t="str">
         <f>'Server Scenarios'!B2:K2</f>
         <v>Version 2019.04.21</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="81" t="s">
-        <v>47</v>
+      <c r="B6" s="96" t="s">
+        <v>46</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="94" t="s">
+      <c r="D6" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="95"/>
-      <c r="F6" s="94" t="s">
+      <c r="E6" s="110"/>
+      <c r="F6" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="96"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="96"/>
-      <c r="J6" s="94" t="s">
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="96"/>
-      <c r="L6" s="96"/>
-      <c r="M6" s="95"/>
+      <c r="K6" s="111"/>
+      <c r="L6" s="111"/>
+      <c r="M6" s="110"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="82"/>
+      <c r="B7" s="97"/>
       <c r="C7" s="3"/>
       <c r="D7" s="13" t="s">
         <v>13</v>
@@ -2802,25 +3152,25 @@
       <c r="E7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="97" t="s">
+      <c r="F7" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="98"/>
-      <c r="H7" s="99" t="s">
+      <c r="G7" s="113"/>
+      <c r="H7" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="98"/>
-      <c r="J7" s="97" t="s">
+      <c r="I7" s="113"/>
+      <c r="J7" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="98"/>
-      <c r="L7" s="99" t="s">
+      <c r="K7" s="113"/>
+      <c r="L7" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="100"/>
+      <c r="M7" s="115"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="82"/>
+      <c r="B8" s="97"/>
       <c r="C8" s="3"/>
       <c r="D8" s="13" t="s">
         <v>8</v>
@@ -2854,7 +3204,7 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="82"/>
+      <c r="B9" s="97"/>
       <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
@@ -2900,7 +3250,7 @@
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="82"/>
+      <c r="B10" s="97"/>
       <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
@@ -2946,7 +3296,7 @@
       </c>
     </row>
     <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="82"/>
+      <c r="B11" s="97"/>
       <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
@@ -2992,32 +3342,32 @@
       </c>
     </row>
     <row r="12" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="82"/>
+      <c r="B12" s="97"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="82"/>
+      <c r="B13" s="97"/>
       <c r="C13" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="87" t="s">
+      <c r="D13" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="88"/>
-      <c r="F13" s="87" t="s">
+      <c r="E13" s="103"/>
+      <c r="F13" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="89"/>
-      <c r="H13" s="89"/>
-      <c r="I13" s="89"/>
-      <c r="J13" s="87" t="s">
+      <c r="G13" s="104"/>
+      <c r="H13" s="104"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="89"/>
-      <c r="L13" s="89"/>
-      <c r="M13" s="88"/>
+      <c r="K13" s="104"/>
+      <c r="L13" s="104"/>
+      <c r="M13" s="103"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="82"/>
+      <c r="B14" s="97"/>
       <c r="C14" s="9"/>
       <c r="D14" s="41" t="s">
         <v>13</v>
@@ -3025,25 +3375,25 @@
       <c r="E14" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="90" t="s">
+      <c r="F14" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="91"/>
-      <c r="H14" s="92" t="s">
+      <c r="G14" s="106"/>
+      <c r="H14" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="91"/>
-      <c r="J14" s="90" t="s">
+      <c r="I14" s="106"/>
+      <c r="J14" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="91"/>
-      <c r="L14" s="92" t="s">
+      <c r="K14" s="106"/>
+      <c r="L14" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="93"/>
+      <c r="M14" s="108"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="82"/>
+      <c r="B15" s="97"/>
       <c r="C15" s="9"/>
       <c r="D15" s="41" t="s">
         <v>8</v>
@@ -3077,7 +3427,7 @@
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="82"/>
+      <c r="B16" s="97"/>
       <c r="C16" s="31" t="s">
         <v>17</v>
       </c>
@@ -3123,7 +3473,7 @@
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="82"/>
+      <c r="B17" s="97"/>
       <c r="C17" s="31" t="s">
         <v>20</v>
       </c>
@@ -3169,7 +3519,7 @@
       </c>
     </row>
     <row r="18" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="83"/>
+      <c r="B18" s="98"/>
       <c r="C18" s="32" t="s">
         <v>19</v>
       </c>
@@ -3216,31 +3566,31 @@
     </row>
     <row r="20" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="84" t="s">
-        <v>48</v>
+      <c r="B21" s="99" t="s">
+        <v>47</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="87" t="s">
+      <c r="D21" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="88"/>
-      <c r="F21" s="87" t="s">
+      <c r="E21" s="103"/>
+      <c r="F21" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="89"/>
-      <c r="H21" s="89"/>
-      <c r="I21" s="88"/>
-      <c r="J21" s="87" t="s">
+      <c r="G21" s="104"/>
+      <c r="H21" s="104"/>
+      <c r="I21" s="103"/>
+      <c r="J21" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="K21" s="89"/>
-      <c r="L21" s="89"/>
-      <c r="M21" s="88"/>
+      <c r="K21" s="104"/>
+      <c r="L21" s="104"/>
+      <c r="M21" s="103"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="85"/>
+      <c r="B22" s="100"/>
       <c r="C22" s="3"/>
       <c r="D22" s="41" t="s">
         <v>13</v>
@@ -3248,25 +3598,25 @@
       <c r="E22" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="90" t="s">
+      <c r="F22" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="91"/>
-      <c r="H22" s="92" t="s">
+      <c r="G22" s="106"/>
+      <c r="H22" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="93"/>
-      <c r="J22" s="90" t="s">
+      <c r="I22" s="108"/>
+      <c r="J22" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="91"/>
-      <c r="L22" s="92" t="s">
+      <c r="K22" s="106"/>
+      <c r="L22" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="M22" s="93"/>
+      <c r="M22" s="108"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="85"/>
+      <c r="B23" s="100"/>
       <c r="C23" s="3"/>
       <c r="D23" s="41" t="s">
         <v>8</v>
@@ -3300,7 +3650,7 @@
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="85"/>
+      <c r="B24" s="100"/>
       <c r="C24" s="4" t="s">
         <v>17</v>
       </c>
@@ -3346,7 +3696,7 @@
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="85"/>
+      <c r="B25" s="100"/>
       <c r="C25" s="4" t="s">
         <v>18</v>
       </c>
@@ -3392,7 +3742,7 @@
       </c>
     </row>
     <row r="26" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="85"/>
+      <c r="B26" s="100"/>
       <c r="C26" s="5" t="s">
         <v>19</v>
       </c>
@@ -3438,7 +3788,7 @@
       </c>
     </row>
     <row r="27" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="85"/>
+      <c r="B27" s="100"/>
       <c r="D27" s="46"/>
       <c r="E27" s="46"/>
       <c r="F27" s="46"/>
@@ -3451,29 +3801,29 @@
       <c r="M27" s="46"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="85"/>
+      <c r="B28" s="100"/>
       <c r="C28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="87" t="s">
+      <c r="D28" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="88"/>
-      <c r="F28" s="87" t="s">
+      <c r="E28" s="103"/>
+      <c r="F28" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="G28" s="89"/>
-      <c r="H28" s="89"/>
-      <c r="I28" s="88"/>
-      <c r="J28" s="87" t="s">
+      <c r="G28" s="104"/>
+      <c r="H28" s="104"/>
+      <c r="I28" s="103"/>
+      <c r="J28" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="K28" s="89"/>
-      <c r="L28" s="89"/>
-      <c r="M28" s="88"/>
+      <c r="K28" s="104"/>
+      <c r="L28" s="104"/>
+      <c r="M28" s="103"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B29" s="85"/>
+      <c r="B29" s="100"/>
       <c r="C29" s="3"/>
       <c r="D29" s="41" t="s">
         <v>13</v>
@@ -3481,25 +3831,25 @@
       <c r="E29" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="F29" s="90" t="s">
+      <c r="F29" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="91"/>
-      <c r="H29" s="92" t="s">
+      <c r="G29" s="106"/>
+      <c r="H29" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="I29" s="93"/>
-      <c r="J29" s="90" t="s">
+      <c r="I29" s="108"/>
+      <c r="J29" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="K29" s="91"/>
-      <c r="L29" s="92" t="s">
+      <c r="K29" s="106"/>
+      <c r="L29" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="M29" s="93"/>
+      <c r="M29" s="108"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="85"/>
+      <c r="B30" s="100"/>
       <c r="C30" s="3"/>
       <c r="D30" s="41" t="s">
         <v>8</v>
@@ -3533,7 +3883,7 @@
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="85"/>
+      <c r="B31" s="100"/>
       <c r="C31" s="4" t="s">
         <v>17</v>
       </c>
@@ -3579,7 +3929,7 @@
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B32" s="85"/>
+      <c r="B32" s="100"/>
       <c r="C32" s="4" t="s">
         <v>20</v>
       </c>
@@ -3625,7 +3975,7 @@
       </c>
     </row>
     <row r="33" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="86"/>
+      <c r="B33" s="101"/>
       <c r="C33" s="5" t="s">
         <v>19</v>
       </c>
@@ -3706,7 +4056,7 @@
     <mergeCell ref="J22:K22"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:M33">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3717,7 +4067,578 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B24151-BCDB-4D54-B778-984CD476EECE}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:K32"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" customWidth="1"/>
+    <col min="9" max="10" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="88" t="str">
+        <f>'Server Scenarios'!B2:K2</f>
+        <v>Version 2019.04.21</v>
+      </c>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="90" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="120" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="121"/>
+      <c r="D6" s="131" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="120" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="121"/>
+      <c r="H6" s="120" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="121"/>
+    </row>
+    <row r="7" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="90"/>
+      <c r="B7" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="50">
+        <v>0</v>
+      </c>
+      <c r="D7" s="131"/>
+      <c r="E7" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="50">
+        <v>0</v>
+      </c>
+      <c r="H7" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="63">
+        <f>Future_Users</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="91"/>
+      <c r="B8" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="52">
+        <v>0</v>
+      </c>
+      <c r="D8" s="131"/>
+      <c r="E8" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="52">
+        <v>0</v>
+      </c>
+      <c r="H8" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="62">
+        <f>Current_Users</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="119" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="128" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="129"/>
+      <c r="E11" s="129"/>
+      <c r="F11" s="130"/>
+      <c r="G11" s="109" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="110"/>
+      <c r="I11" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" s="110"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="97"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="117"/>
+      <c r="E12" s="117"/>
+      <c r="F12" s="118"/>
+      <c r="G12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="97"/>
+      <c r="C13" s="122" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="123"/>
+      <c r="E13" s="123"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="33">
+        <f>IF(Current_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Current_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="35">
+        <f>G13*(1+VM_OVERHEAD)</f>
+        <v>1.2</v>
+      </c>
+      <c r="I13" s="33">
+        <f>IF(Current_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Current_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
+        <v>1</v>
+      </c>
+      <c r="J13" s="35">
+        <f>I13*(1+VM_OVERHEAD)</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="97"/>
+      <c r="C14" s="122" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="123"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="33">
+        <f>IF(Current_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_RAM, IF(Current_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_RAM,PROXY_MEDIUM_RAM))</f>
+        <v>2</v>
+      </c>
+      <c r="H14" s="35">
+        <f>G14*(1+VM_OVERHEAD)</f>
+        <v>2.4</v>
+      </c>
+      <c r="I14" s="33">
+        <f>G14+(Current_BranchTip)</f>
+        <v>2</v>
+      </c>
+      <c r="J14" s="35">
+        <f>I14*(1+VM_OVERHEAD)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="97"/>
+      <c r="C15" s="125" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="126"/>
+      <c r="E15" s="126"/>
+      <c r="F15" s="127"/>
+      <c r="G15" s="34">
+        <f>Current_BranchTip</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="47">
+        <f>G15</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="34">
+        <f>Current_Storage*GVFS_SCALE_FACTOR</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="47">
+        <f>I15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="97"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="97"/>
+      <c r="C17" s="128" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="129"/>
+      <c r="E17" s="129"/>
+      <c r="F17" s="130"/>
+      <c r="G17" s="109" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="110"/>
+      <c r="I17" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="110"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="97"/>
+      <c r="C18" s="116"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="118"/>
+      <c r="G18" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" s="42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="97"/>
+      <c r="C19" s="122" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="123"/>
+      <c r="E19" s="123"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="33">
+        <f>IF(Future_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Future_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="35">
+        <f>G19*(1+VM_OVERHEAD)</f>
+        <v>1.2</v>
+      </c>
+      <c r="I19" s="33">
+        <f>IF(Future_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Future_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
+        <v>1</v>
+      </c>
+      <c r="J19" s="35">
+        <f>I19*(1+VM_OVERHEAD)</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="97"/>
+      <c r="C20" s="122" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="123"/>
+      <c r="E20" s="123"/>
+      <c r="F20" s="124"/>
+      <c r="G20" s="33">
+        <f>IF(Future_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_RAM, IF(Future_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_RAM,PROXY_MEDIUM_RAM))</f>
+        <v>2</v>
+      </c>
+      <c r="H20" s="35">
+        <f>G20*(1+VM_OVERHEAD)</f>
+        <v>2.4</v>
+      </c>
+      <c r="I20" s="33">
+        <f>G20+Future_BranchTip</f>
+        <v>2</v>
+      </c>
+      <c r="J20" s="35">
+        <f>I20*(1+VM_OVERHEAD)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="98"/>
+      <c r="C21" s="125" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="126"/>
+      <c r="E21" s="126"/>
+      <c r="F21" s="127"/>
+      <c r="G21" s="34">
+        <f>Future_BranchTip</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="47">
+        <f>G21</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="34">
+        <f>Future_Storage*GVFS_SCALE_FACTOR</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="47">
+        <f>I21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="73" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="75"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="66"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="67"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="69"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="67"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="68"/>
+      <c r="K26" s="69"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="67"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="67"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="68"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="68"/>
+      <c r="J28" s="68"/>
+      <c r="K28" s="69"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="67"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="68"/>
+      <c r="J29" s="68"/>
+      <c r="K29" s="69"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="67"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="68"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="68"/>
+      <c r="H30" s="68"/>
+      <c r="I30" s="68"/>
+      <c r="J30" s="68"/>
+      <c r="K30" s="69"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B31" s="67"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="68"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="68"/>
+      <c r="H31" s="68"/>
+      <c r="I31" s="68"/>
+      <c r="J31" s="68"/>
+      <c r="K31" s="69"/>
+    </row>
+    <row r="32" spans="2:11" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="70"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="71"/>
+      <c r="K32" s="72"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="23">
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="B23:K23"/>
+    <mergeCell ref="B24:K32"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B11:B21"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C21:F21"/>
+  </mergeCells>
+  <conditionalFormatting sqref="G10:H10">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18:H21 G12:H16">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:H11">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17:H17">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12:J12 J13:J15">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11:J11">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18:J18 J19:J21">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19:I21">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17:J17">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13:I15">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>Current_Storage&lt;=Future_Storage</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>Current_BranchTip &lt;= Future_BranchTip</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9C01BD-A0E7-4C75-963D-65D4B351A825}">
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
@@ -3737,607 +4658,362 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="73" t="str">
+      <c r="B2" s="88" t="str">
         <f>'Server Scenarios'!B2:K2</f>
         <v>Version 2019.04.21</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="75" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="105" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="106"/>
-      <c r="D7" s="116" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="105" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="106"/>
-      <c r="H7" s="105" t="s">
+      <c r="A7" s="90" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="120" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="121"/>
+      <c r="E7" s="120" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="121"/>
+    </row>
+    <row r="8" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="90"/>
+      <c r="B8" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="50">
+        <v>0</v>
+      </c>
+      <c r="E8" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="I7" s="106"/>
-    </row>
-    <row r="8" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="75"/>
-      <c r="B8" s="50" t="s">
+      <c r="F8" s="63">
+        <f>Future_Users</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="91"/>
+      <c r="B9" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="51">
-        <v>0</v>
-      </c>
-      <c r="D8" s="116"/>
-      <c r="E8" s="50" t="s">
+      <c r="C9" s="52">
+        <v>0</v>
+      </c>
+      <c r="E9" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="51">
-        <v>0</v>
-      </c>
-      <c r="H8" s="50" t="s">
-        <v>78</v>
-      </c>
-      <c r="I8" s="118">
-        <f>Future_Users</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="76"/>
-      <c r="B9" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="53">
-        <v>0</v>
-      </c>
-      <c r="D9" s="116"/>
-      <c r="E9" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="51">
-        <v>0</v>
-      </c>
-      <c r="H9" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="117">
+      <c r="F9" s="62">
         <f>Current_Users</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E10" s="52" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="119" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="128" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="129"/>
+      <c r="E12" s="129"/>
+      <c r="F12" s="130"/>
+      <c r="G12" s="109" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="110"/>
+    </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="104" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="113" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="114"/>
-      <c r="E13" s="114"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="94" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="95"/>
+      <c r="B13" s="97"/>
+      <c r="C13" s="116"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="118"/>
+      <c r="G13" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="82"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="102"/>
-      <c r="E14" s="102"/>
-      <c r="F14" s="103"/>
-      <c r="G14" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="82"/>
-      <c r="C15" s="107" t="s">
+      <c r="B14" s="97"/>
+      <c r="C14" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="108"/>
-      <c r="E15" s="108"/>
-      <c r="F15" s="109"/>
-      <c r="G15" s="33">
+      <c r="D14" s="123"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="33">
         <f>IF(Current_Users&gt;CS_LOW_USERS,CS_HIGH_CORES,CS_LOW_CORES)</f>
         <v>2</v>
       </c>
+      <c r="H14" s="35">
+        <f>G14*(1+VM_OVERHEAD)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="97"/>
+      <c r="C15" s="122" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="123"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="33">
+        <f>IF(Current_Users&gt;CS_LOW_USERS,CS_HIGH_RAM,CS_LOW_RAM)</f>
+        <v>8</v>
+      </c>
       <c r="H15" s="35">
         <f>G15*(1+VM_OVERHEAD)</f>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="82"/>
-      <c r="C16" s="107" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="108"/>
-      <c r="E16" s="108"/>
-      <c r="F16" s="109"/>
-      <c r="G16" s="33">
-        <f>IF(Current_Users&gt;CS_LOW_USERS,CS_HIGH_RAM,CS_LOW_RAM)</f>
-        <v>8</v>
-      </c>
-      <c r="H16" s="35">
-        <f>G16*(1+VM_OVERHEAD)</f>
         <v>9.6</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="82"/>
-      <c r="C17" s="110" t="s">
+    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="97"/>
+      <c r="C16" s="125" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="111"/>
-      <c r="E17" s="111"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="34">
+      <c r="D16" s="126"/>
+      <c r="E16" s="126"/>
+      <c r="F16" s="127"/>
+      <c r="G16" s="34">
         <f>Current_Storage*CS_STORAGE_FACTOR</f>
         <v>0</v>
       </c>
-      <c r="H17" s="47">
-        <f>G17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="82"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="82"/>
-      <c r="C19" s="113" t="s">
+      <c r="H16" s="47">
+        <f>G16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="97"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="97"/>
+      <c r="C18" s="128" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="114"/>
-      <c r="E19" s="114"/>
-      <c r="F19" s="115"/>
-      <c r="G19" s="94" t="s">
-        <v>54</v>
-      </c>
-      <c r="H19" s="95"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="82"/>
-      <c r="C20" s="101"/>
-      <c r="D20" s="102"/>
-      <c r="E20" s="102"/>
-      <c r="F20" s="103"/>
-      <c r="G20" s="41" t="s">
+      <c r="D18" s="129"/>
+      <c r="E18" s="129"/>
+      <c r="F18" s="130"/>
+      <c r="G18" s="109" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="110"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="97"/>
+      <c r="C19" s="116"/>
+      <c r="D19" s="117"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="118"/>
+      <c r="G19" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="42" t="s">
+      <c r="H19" s="42" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="82"/>
-      <c r="C21" s="107" t="s">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="97"/>
+      <c r="C20" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="108"/>
-      <c r="E21" s="108"/>
-      <c r="F21" s="109"/>
-      <c r="G21" s="33">
+      <c r="D20" s="123"/>
+      <c r="E20" s="123"/>
+      <c r="F20" s="124"/>
+      <c r="G20" s="33">
         <f>IF(Future_Users&gt;CS_LOW_USERS,CS_HIGH_CORES,CS_LOW_CORES)</f>
         <v>2</v>
       </c>
+      <c r="H20" s="35">
+        <f>G20*(1+VM_OVERHEAD)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="97"/>
+      <c r="C21" s="122" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="123"/>
+      <c r="E21" s="123"/>
+      <c r="F21" s="124"/>
+      <c r="G21" s="33">
+        <f>IF(Future_Users&gt;CS_LOW_USERS,CS_HIGH_RAM,CS_LOW_RAM)</f>
+        <v>8</v>
+      </c>
       <c r="H21" s="35">
         <f>G21*(1+VM_OVERHEAD)</f>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="82"/>
-      <c r="C22" s="107" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="108"/>
-      <c r="E22" s="108"/>
-      <c r="F22" s="109"/>
-      <c r="G22" s="33">
-        <f>IF(Future_Users&gt;CS_LOW_USERS,CS_HIGH_RAM,CS_LOW_RAM)</f>
-        <v>8</v>
-      </c>
-      <c r="H22" s="35">
-        <f>G22*(1+VM_OVERHEAD)</f>
         <v>9.6</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="83"/>
-      <c r="C23" s="110" t="s">
+    <row r="22" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="98"/>
+      <c r="C22" s="125" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="111"/>
-      <c r="E23" s="111"/>
-      <c r="F23" s="112"/>
-      <c r="G23" s="34">
+      <c r="D22" s="126"/>
+      <c r="E22" s="126"/>
+      <c r="F22" s="127"/>
+      <c r="G22" s="34">
         <f>Future_Storage*CS_STORAGE_FACTOR</f>
         <v>0</v>
       </c>
-      <c r="H23" s="47">
-        <f>G23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B25" s="104" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="113" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="114"/>
-      <c r="E25" s="114"/>
-      <c r="F25" s="115"/>
-      <c r="G25" s="94" t="s">
-        <v>54</v>
-      </c>
-      <c r="H25" s="95"/>
-      <c r="I25" s="94" t="s">
-        <v>61</v>
-      </c>
-      <c r="J25" s="95"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B26" s="82"/>
-      <c r="C26" s="101"/>
-      <c r="D26" s="102"/>
-      <c r="E26" s="102"/>
-      <c r="F26" s="103"/>
-      <c r="G26" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I26" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="J26" s="42" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="82"/>
-      <c r="C27" s="107" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="108"/>
-      <c r="E27" s="108"/>
-      <c r="F27" s="109"/>
-      <c r="G27" s="33">
-        <f>IF(Current_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Current_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
-        <v>1</v>
-      </c>
-      <c r="H27" s="35">
-        <f>G27*(1+VM_OVERHEAD)</f>
-        <v>1.2</v>
-      </c>
-      <c r="I27" s="33">
-        <f>IF(Current_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Current_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
-        <v>1</v>
-      </c>
-      <c r="J27" s="35">
-        <f>I27*(1+VM_OVERHEAD)</f>
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="82"/>
-      <c r="C28" s="107" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="108"/>
-      <c r="E28" s="108"/>
-      <c r="F28" s="109"/>
-      <c r="G28" s="33">
-        <f>IF(Current_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_RAM, IF(Current_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_RAM,PROXY_MEDIUM_RAM))</f>
-        <v>2</v>
-      </c>
-      <c r="H28" s="35">
-        <f>G28*(1+VM_OVERHEAD)</f>
-        <v>2.4</v>
-      </c>
-      <c r="I28" s="33">
-        <f>G28+(Current_BranchTip)</f>
-        <v>2</v>
-      </c>
-      <c r="J28" s="35">
-        <f>I28*(1+VM_OVERHEAD)</f>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="82"/>
-      <c r="C29" s="110" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="111"/>
-      <c r="E29" s="111"/>
-      <c r="F29" s="112"/>
-      <c r="G29" s="34">
-        <f>Current_BranchTip*Active_Branches</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="47">
-        <f>G29</f>
-        <v>0</v>
-      </c>
-      <c r="I29" s="34">
-        <f>Current_Storage*GVFS_SCALE_FACTOR</f>
-        <v>0</v>
-      </c>
-      <c r="J29" s="47">
-        <f>I29</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="82"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B31" s="82"/>
-      <c r="C31" s="113" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="114"/>
-      <c r="E31" s="114"/>
-      <c r="F31" s="115"/>
-      <c r="G31" s="94" t="s">
-        <v>54</v>
-      </c>
-      <c r="H31" s="95"/>
-      <c r="I31" s="94" t="s">
-        <v>61</v>
-      </c>
-      <c r="J31" s="95"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B32" s="82"/>
-      <c r="C32" s="101"/>
-      <c r="D32" s="102"/>
-      <c r="E32" s="102"/>
-      <c r="F32" s="103"/>
-      <c r="G32" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="H32" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="I32" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="J32" s="42" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B33" s="82"/>
-      <c r="C33" s="107" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" s="108"/>
-      <c r="E33" s="108"/>
-      <c r="F33" s="109"/>
-      <c r="G33" s="33">
-        <f>IF(Future_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Future_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
-        <v>1</v>
-      </c>
-      <c r="H33" s="35">
-        <f>G33*(1+VM_OVERHEAD)</f>
-        <v>1.2</v>
-      </c>
-      <c r="I33" s="33">
-        <f>IF(Future_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Future_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
-        <v>1</v>
-      </c>
-      <c r="J33" s="35">
-        <f>I33*(1+VM_OVERHEAD)</f>
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B34" s="82"/>
-      <c r="C34" s="107" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="108"/>
-      <c r="E34" s="108"/>
-      <c r="F34" s="109"/>
-      <c r="G34" s="33">
-        <f>IF(Future_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_RAM, IF(Future_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_RAM,PROXY_MEDIUM_RAM))</f>
-        <v>2</v>
-      </c>
-      <c r="H34" s="35">
-        <f>G34*(1+VM_OVERHEAD)</f>
-        <v>2.4</v>
-      </c>
-      <c r="I34" s="33">
-        <f>G34+Future_BranchTip</f>
-        <v>2</v>
-      </c>
-      <c r="J34" s="35">
-        <f>I34*(1+VM_OVERHEAD)</f>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="83"/>
-      <c r="C35" s="110" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" s="111"/>
-      <c r="E35" s="111"/>
-      <c r="F35" s="112"/>
-      <c r="G35" s="34">
-        <f>Future_BranchTip*Active_Branches</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="47">
-        <f>G35</f>
-        <v>0</v>
-      </c>
-      <c r="I35" s="34">
-        <f>Future_Storage*GVFS_SCALE_FACTOR</f>
-        <v>0</v>
-      </c>
-      <c r="J35" s="47">
-        <f>I35</f>
-        <v>0</v>
-      </c>
+      <c r="H22" s="47">
+        <f>G22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="73" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="74"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="74"/>
+      <c r="K24" s="75"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="64" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="65"/>
+      <c r="K25" s="66"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="67"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="68"/>
+      <c r="K26" s="69"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="67"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="67"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="68"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="68"/>
+      <c r="J28" s="68"/>
+      <c r="K28" s="69"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="67"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="68"/>
+      <c r="J29" s="68"/>
+      <c r="K29" s="69"/>
+    </row>
+    <row r="30" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="70"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="72"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="34">
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="H7:I7"/>
+  <mergeCells count="19">
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="B24:K24"/>
+    <mergeCell ref="B25:K30"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="B12:B22"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C14:F14"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="G18:H18"/>
     <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B25:B35"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C29:F29"/>
   </mergeCells>
-  <conditionalFormatting sqref="G13:H24">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+  <conditionalFormatting sqref="G12:H23">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
       <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G32:H35 G26:H30">
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G25:H25">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G31:H31">
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I26:J26 J27:J29">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I25:J25">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32:J32 J33:J35">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I33:I35">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31:J31">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I27:I29">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>Current_Storage&lt;=Future_Storage</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>Current_BranchTip &lt;= Future_BranchTip</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4457,11 +5133,11 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{312B28CD-EB51-4560-8E58-B9E03DAFD80D}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="d4f1fd26-cd3f-48df-8559-6269d85163e3"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>

</xml_diff>